<commit_message>
v2 result in 0827
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="47">
   <si>
     <t>20210618</t>
   </si>
@@ -119,6 +119,9 @@
     <t>20220128</t>
   </si>
   <si>
+    <t>20220204</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -150,6 +153,9 @@
   </si>
   <si>
     <t>20210813-20210820</t>
+  </si>
+  <si>
+    <t>20210820-20210827</t>
   </si>
   <si>
     <t>SUM</t>
@@ -510,15 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -619,10 +625,13 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -697,9 +706,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -774,9 +783,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -851,9 +860,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -928,9 +937,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1005,9 +1014,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1082,9 +1091,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1159,9 +1168,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1236,9 +1245,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1313,9 +1322,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1390,107 +1399,187 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="M12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="N12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="O12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="P12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Q12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="R12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="S12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="T12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="U12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="V12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="W12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="X12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Y12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Z12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AA12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AB12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AC12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AD12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AE12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AF12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AG12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AH12">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AI12">
+        <v>837074.2362500001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C13">
         <v>1879592.178333333</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>2819388.2675</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>3759184.356666667</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>4801479.284583334</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>5843774.2125</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>6886069.140416667</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>7928364.068333333</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>8765438.304583333</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>9602512.540833334</v>
       </c>
-      <c r="L12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="M12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="N12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="O12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="P12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="Q12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="R12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="S12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="T12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="U12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="V12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="W12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="X12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="Y12">
-        <v>9602512.540833334</v>
-      </c>
-      <c r="Z12">
-        <v>8662716.451666666</v>
-      </c>
-      <c r="AA12">
-        <v>7722920.3625</v>
-      </c>
-      <c r="AB12">
-        <v>6783124.273333333</v>
-      </c>
-      <c r="AC12">
-        <v>5843328.184166666</v>
-      </c>
-      <c r="AD12">
-        <v>4801033.25625</v>
-      </c>
-      <c r="AE12">
-        <v>3758738.328333333</v>
-      </c>
-      <c r="AF12">
-        <v>2716443.400416667</v>
-      </c>
-      <c r="AG12">
+      <c r="L13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="M13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="N13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="O13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="P13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="Q13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="R13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="S13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="T13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="U13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="V13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="W13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="X13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="Y13">
+        <v>10439586.77708333</v>
+      </c>
+      <c r="Z13">
+        <v>9499790.687916666</v>
+      </c>
+      <c r="AA13">
+        <v>8559994.598749999</v>
+      </c>
+      <c r="AB13">
+        <v>7620198.509583334</v>
+      </c>
+      <c r="AC13">
+        <v>6680402.420416666</v>
+      </c>
+      <c r="AD13">
+        <v>5638107.4925</v>
+      </c>
+      <c r="AE13">
+        <v>4595812.564583333</v>
+      </c>
+      <c r="AF13">
+        <v>3553517.636666667</v>
+      </c>
+      <c r="AG13">
+        <v>2511222.70875</v>
+      </c>
+      <c r="AH13">
         <v>1674148.4725</v>
       </c>
-      <c r="AH12">
+      <c r="AI13">
         <v>837074.2362500001</v>
       </c>
     </row>
@@ -1501,15 +1590,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1610,10 +1699,13 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -1688,9 +1780,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -1765,9 +1857,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -1842,9 +1934,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -1919,9 +2011,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -1996,9 +2088,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2073,9 +2165,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2150,9 +2242,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2227,9 +2319,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2304,9 +2396,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2381,107 +2473,187 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>981750</v>
+      </c>
+      <c r="M12">
+        <v>981750</v>
+      </c>
+      <c r="N12">
+        <v>981750</v>
+      </c>
+      <c r="O12">
+        <v>981750</v>
+      </c>
+      <c r="P12">
+        <v>981750</v>
+      </c>
+      <c r="Q12">
+        <v>981750</v>
+      </c>
+      <c r="R12">
+        <v>981750</v>
+      </c>
+      <c r="S12">
+        <v>981750</v>
+      </c>
+      <c r="T12">
+        <v>981750</v>
+      </c>
+      <c r="U12">
+        <v>981750</v>
+      </c>
+      <c r="V12">
+        <v>981750</v>
+      </c>
+      <c r="W12">
+        <v>981750</v>
+      </c>
+      <c r="X12">
+        <v>981750</v>
+      </c>
+      <c r="Y12">
+        <v>981750</v>
+      </c>
+      <c r="Z12">
+        <v>981750</v>
+      </c>
+      <c r="AA12">
+        <v>981750</v>
+      </c>
+      <c r="AB12">
+        <v>981750</v>
+      </c>
+      <c r="AC12">
+        <v>981750</v>
+      </c>
+      <c r="AD12">
+        <v>981750</v>
+      </c>
+      <c r="AE12">
+        <v>981750</v>
+      </c>
+      <c r="AF12">
+        <v>981750</v>
+      </c>
+      <c r="AG12">
+        <v>981750</v>
+      </c>
+      <c r="AH12">
+        <v>981750</v>
+      </c>
+      <c r="AI12">
+        <v>981750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
         <v>942083.3333333334</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>1829625</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>2717166.666666667</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>3604708.333333333</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>4477375</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>5350041.666666667</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>6222708.333333334</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>7095375.000000001</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>8022583.333333334</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>9004333.333333334</v>
       </c>
-      <c r="L12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="M12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="N12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="O12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="P12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="Q12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="R12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="S12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="T12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="U12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="V12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="W12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="X12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="Y12">
-        <v>9004333.333333334</v>
-      </c>
-      <c r="Z12">
-        <v>8062250</v>
-      </c>
-      <c r="AA12">
-        <v>7174708.333333333</v>
-      </c>
-      <c r="AB12">
-        <v>6287166.666666666</v>
-      </c>
-      <c r="AC12">
-        <v>5399625</v>
-      </c>
-      <c r="AD12">
-        <v>4526958.333333334</v>
-      </c>
-      <c r="AE12">
-        <v>3654291.666666667</v>
-      </c>
-      <c r="AF12">
-        <v>2781625</v>
-      </c>
-      <c r="AG12">
-        <v>1908958.333333333</v>
-      </c>
-      <c r="AH12">
+      <c r="L13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="M13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="N13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="O13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="P13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="Q13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="R13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="S13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="T13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="U13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="V13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="W13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="X13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="Y13">
+        <v>9986083.333333334</v>
+      </c>
+      <c r="Z13">
+        <v>9044000</v>
+      </c>
+      <c r="AA13">
+        <v>8156458.333333333</v>
+      </c>
+      <c r="AB13">
+        <v>7268916.666666666</v>
+      </c>
+      <c r="AC13">
+        <v>6381375</v>
+      </c>
+      <c r="AD13">
+        <v>5508708.333333334</v>
+      </c>
+      <c r="AE13">
+        <v>4636041.666666666</v>
+      </c>
+      <c r="AF13">
+        <v>3763375</v>
+      </c>
+      <c r="AG13">
+        <v>2890708.333333333</v>
+      </c>
+      <c r="AH13">
+        <v>1963500</v>
+      </c>
+      <c r="AI13">
         <v>981750</v>
       </c>
     </row>
@@ -2492,15 +2664,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2601,10 +2773,13 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -2679,9 +2854,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -2756,9 +2931,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -2833,9 +3008,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -2910,9 +3085,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -2987,9 +3162,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3064,9 +3239,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -3141,9 +3316,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -3218,9 +3393,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -3295,9 +3470,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -3372,107 +3547,187 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="M12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="N12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="O12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="P12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Q12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="R12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="S12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="T12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="U12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="V12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="W12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="X12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Y12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Z12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AA12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AB12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AC12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AD12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AE12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AF12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AG12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AH12">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AI12">
+        <v>2022976.932083334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C13">
         <v>4045953.864166667</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>6068930.796250001</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>8091907.728333334</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>10114884.66041667</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>12137861.5925</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>14160838.52458333</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>16183815.45666667</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>18206792.38875</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>20229769.32083334</v>
       </c>
-      <c r="L12">
+      <c r="L13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="M13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="N13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="O13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="P13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="Q13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="R13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="S13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="T13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="U13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="V13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="W13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="X13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="Y13">
+        <v>22252746.25291667</v>
+      </c>
+      <c r="Z13">
         <v>20229769.32083334</v>
       </c>
-      <c r="M12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="N12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="O12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="P12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="Q12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="R12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="S12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="T12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="U12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="V12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="W12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="X12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="Y12">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="Z12">
+      <c r="AA13">
         <v>18206792.38875</v>
       </c>
-      <c r="AA12">
+      <c r="AB13">
         <v>16183815.45666667</v>
       </c>
-      <c r="AB12">
+      <c r="AC13">
         <v>14160838.52458333</v>
       </c>
-      <c r="AC12">
+      <c r="AD13">
         <v>12137861.5925</v>
       </c>
-      <c r="AD12">
+      <c r="AE13">
         <v>10114884.66041667</v>
       </c>
-      <c r="AE12">
+      <c r="AF13">
         <v>8091907.728333334</v>
       </c>
-      <c r="AF12">
+      <c r="AG13">
         <v>6068930.796250001</v>
       </c>
-      <c r="AG12">
+      <c r="AH13">
         <v>4045953.864166667</v>
       </c>
-      <c r="AH12">
+      <c r="AI13">
         <v>2022976.932083334</v>
       </c>
     </row>
@@ -3483,15 +3738,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3592,10 +3847,13 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -3670,9 +3928,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -3747,9 +4005,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -3824,9 +4082,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -3901,9 +4159,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -3978,9 +4236,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -4055,9 +4313,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -4132,9 +4390,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -4209,9 +4467,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -4286,9 +4544,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -4363,107 +4621,187 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="M12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="N12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="O12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="P12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Q12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="R12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="S12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="T12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="U12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="V12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="W12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="X12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Y12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Z12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AA12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AB12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AC12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AD12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AE12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AF12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AG12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AH12">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AI12">
+        <v>5319315.755833333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C13">
         <v>10638631.51166667</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>15957947.2675</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>21277263.02333333</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>26596578.77916667</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>31915894.535</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>37235210.29083334</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>42554526.04666667</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>47873841.80250001</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>53193157.55833334</v>
       </c>
-      <c r="L12">
+      <c r="L13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="M13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="N13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="O13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="P13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="Q13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="R13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="S13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="T13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="U13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="V13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="W13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="X13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="Y13">
+        <v>58512473.31416668</v>
+      </c>
+      <c r="Z13">
         <v>53193157.55833334</v>
       </c>
-      <c r="M12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="N12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="O12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="P12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="Q12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="R12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="S12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="T12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="U12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="V12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="W12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="X12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="Y12">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="Z12">
+      <c r="AA13">
         <v>47873841.80250001</v>
       </c>
-      <c r="AA12">
+      <c r="AB13">
         <v>42554526.04666667</v>
       </c>
-      <c r="AB12">
+      <c r="AC13">
         <v>37235210.29083334</v>
       </c>
-      <c r="AC12">
+      <c r="AD13">
         <v>31915894.535</v>
       </c>
-      <c r="AD12">
+      <c r="AE13">
         <v>26596578.77916667</v>
       </c>
-      <c r="AE12">
+      <c r="AF13">
         <v>21277263.02333333</v>
       </c>
-      <c r="AF12">
+      <c r="AG13">
         <v>15957947.2675</v>
       </c>
-      <c r="AG12">
+      <c r="AH13">
         <v>10638631.51166667</v>
       </c>
-      <c r="AH12">
+      <c r="AI13">
         <v>5319315.755833333</v>
       </c>
     </row>
@@ -4474,15 +4812,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4583,10 +4921,13 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -4661,9 +5002,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -4738,9 +5079,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -4815,9 +5156,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -4892,9 +5233,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -4969,9 +5310,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -5046,9 +5387,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -5123,9 +5464,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -5200,9 +5541,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -5277,9 +5618,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -5354,107 +5695,187 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="M12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="N12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="O12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="P12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Q12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="R12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="S12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="T12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="U12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="V12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="W12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="X12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Y12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Z12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AA12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AB12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AC12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AD12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AE12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AF12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AG12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AH12">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AI12">
+        <v>2833161790.824167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C13">
         <v>5666323581.648334</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>8499485372.4725</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>11332647163.29667</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>14165808954.12083</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>16998970744.945</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>19832132535.76917</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>22665294326.59333</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>25498456117.4175</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>28331617908.24166</v>
       </c>
-      <c r="L12">
+      <c r="L13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="M13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="N13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="O13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="P13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="Q13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="R13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="S13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="T13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="U13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="V13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="W13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="X13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="Y13">
+        <v>31164779699.06583</v>
+      </c>
+      <c r="Z13">
         <v>28331617908.24166</v>
       </c>
-      <c r="M12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="N12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="O12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="P12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="Q12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="R12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="S12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="T12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="U12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="V12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="W12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="X12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="Y12">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="Z12">
+      <c r="AA13">
         <v>25498456117.4175</v>
       </c>
-      <c r="AA12">
+      <c r="AB13">
         <v>22665294326.59333</v>
       </c>
-      <c r="AB12">
+      <c r="AC13">
         <v>19832132535.76917</v>
       </c>
-      <c r="AC12">
+      <c r="AD13">
         <v>16998970744.945</v>
       </c>
-      <c r="AD12">
+      <c r="AE13">
         <v>14165808954.12083</v>
       </c>
-      <c r="AE12">
+      <c r="AF13">
         <v>11332647163.29667</v>
       </c>
-      <c r="AF12">
+      <c r="AG13">
         <v>8499485372.4725</v>
       </c>
-      <c r="AG12">
+      <c r="AH13">
         <v>5666323581.648334</v>
       </c>
-      <c r="AH12">
+      <c r="AI13">
         <v>2833161790.824167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2 result in 0903
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="49">
   <si>
     <t>20210618</t>
   </si>
@@ -122,6 +122,9 @@
     <t>20220204</t>
   </si>
   <si>
+    <t>20220211</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -156,6 +159,9 @@
   </si>
   <si>
     <t>20210820-20210827</t>
+  </si>
+  <si>
+    <t>20210827-20210903</t>
   </si>
   <si>
     <t>SUM</t>
@@ -516,15 +522,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -628,10 +634,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -706,9 +715,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -783,9 +792,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -860,9 +869,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -937,9 +946,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1014,9 +1023,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1091,9 +1100,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1168,9 +1177,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1245,9 +1254,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1322,9 +1331,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1399,9 +1408,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1476,110 +1485,190 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C13">
+        <v>47</v>
+      </c>
+      <c r="M13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="N13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="O13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="P13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Q13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="R13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="S13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="T13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="U13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="V13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="W13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="X13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Y13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="Z13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AA13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AB13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AC13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AD13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AE13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AF13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AG13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AH13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AI13">
+        <v>837074.2362500001</v>
+      </c>
+      <c r="AJ13">
+        <v>837074.2362500001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C14">
         <v>1879592.178333333</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>2819388.2675</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>3759184.356666667</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>4801479.284583334</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>5843774.2125</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>6886069.140416667</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>7928364.068333333</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>8765438.304583333</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>9602512.540833334</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>10439586.77708333</v>
       </c>
-      <c r="M13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="N13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="O13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="P13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="Q13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="R13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="S13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="T13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="U13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="V13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="W13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="X13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="Y13">
-        <v>10439586.77708333</v>
-      </c>
-      <c r="Z13">
-        <v>9499790.687916666</v>
-      </c>
-      <c r="AA13">
-        <v>8559994.598749999</v>
-      </c>
-      <c r="AB13">
-        <v>7620198.509583334</v>
-      </c>
-      <c r="AC13">
-        <v>6680402.420416666</v>
-      </c>
-      <c r="AD13">
-        <v>5638107.4925</v>
-      </c>
-      <c r="AE13">
-        <v>4595812.564583333</v>
-      </c>
-      <c r="AF13">
-        <v>3553517.636666667</v>
-      </c>
-      <c r="AG13">
+      <c r="M14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="N14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="O14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="P14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="Q14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="R14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="S14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="T14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="U14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="V14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="W14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="X14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="Y14">
+        <v>11276661.01333333</v>
+      </c>
+      <c r="Z14">
+        <v>10336864.92416667</v>
+      </c>
+      <c r="AA14">
+        <v>9397068.834999999</v>
+      </c>
+      <c r="AB14">
+        <v>8457272.745833334</v>
+      </c>
+      <c r="AC14">
+        <v>7517476.656666666</v>
+      </c>
+      <c r="AD14">
+        <v>6475181.72875</v>
+      </c>
+      <c r="AE14">
+        <v>5432886.800833333</v>
+      </c>
+      <c r="AF14">
+        <v>4390591.872916667</v>
+      </c>
+      <c r="AG14">
+        <v>3348296.945</v>
+      </c>
+      <c r="AH14">
         <v>2511222.70875</v>
       </c>
-      <c r="AH13">
+      <c r="AI14">
         <v>1674148.4725</v>
       </c>
-      <c r="AI13">
+      <c r="AJ14">
         <v>837074.2362500001</v>
       </c>
     </row>
@@ -1590,15 +1679,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1702,10 +1791,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -1780,9 +1872,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -1857,9 +1949,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -1934,9 +2026,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2011,9 +2103,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2088,9 +2180,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2165,9 +2257,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2242,9 +2334,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2319,9 +2411,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2396,9 +2488,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2473,9 +2565,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -2550,110 +2642,190 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
+        <v>47</v>
+      </c>
+      <c r="M13">
+        <v>981750</v>
+      </c>
+      <c r="N13">
+        <v>981750</v>
+      </c>
+      <c r="O13">
+        <v>981750</v>
+      </c>
+      <c r="P13">
+        <v>981750</v>
+      </c>
+      <c r="Q13">
+        <v>981750</v>
+      </c>
+      <c r="R13">
+        <v>981750</v>
+      </c>
+      <c r="S13">
+        <v>981750</v>
+      </c>
+      <c r="T13">
+        <v>981750</v>
+      </c>
+      <c r="U13">
+        <v>981750</v>
+      </c>
+      <c r="V13">
+        <v>981750</v>
+      </c>
+      <c r="W13">
+        <v>981750</v>
+      </c>
+      <c r="X13">
+        <v>981750</v>
+      </c>
+      <c r="Y13">
+        <v>981750</v>
+      </c>
+      <c r="Z13">
+        <v>981750</v>
+      </c>
+      <c r="AA13">
+        <v>981750</v>
+      </c>
+      <c r="AB13">
+        <v>981750</v>
+      </c>
+      <c r="AC13">
+        <v>981750</v>
+      </c>
+      <c r="AD13">
+        <v>981750</v>
+      </c>
+      <c r="AE13">
+        <v>981750</v>
+      </c>
+      <c r="AF13">
+        <v>981750</v>
+      </c>
+      <c r="AG13">
+        <v>981750</v>
+      </c>
+      <c r="AH13">
+        <v>981750</v>
+      </c>
+      <c r="AI13">
+        <v>981750</v>
+      </c>
+      <c r="AJ13">
+        <v>981750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
         <v>942083.3333333334</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>1829625</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>2717166.666666667</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>3604708.333333333</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>4477375</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>5350041.666666667</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>6222708.333333334</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>7095375.000000001</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>8022583.333333334</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>9004333.333333334</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>9986083.333333334</v>
       </c>
-      <c r="M13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="N13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="O13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="P13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="Q13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="R13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="S13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="T13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="U13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="V13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="W13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="X13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="Y13">
-        <v>9986083.333333334</v>
-      </c>
-      <c r="Z13">
-        <v>9044000</v>
-      </c>
-      <c r="AA13">
-        <v>8156458.333333333</v>
-      </c>
-      <c r="AB13">
-        <v>7268916.666666666</v>
-      </c>
-      <c r="AC13">
-        <v>6381375</v>
-      </c>
-      <c r="AD13">
-        <v>5508708.333333334</v>
-      </c>
-      <c r="AE13">
-        <v>4636041.666666666</v>
-      </c>
-      <c r="AF13">
-        <v>3763375</v>
-      </c>
-      <c r="AG13">
-        <v>2890708.333333333</v>
-      </c>
-      <c r="AH13">
+      <c r="M14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="N14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="O14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="P14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="Q14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="R14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="S14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="T14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="U14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="V14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="W14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="X14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="Y14">
+        <v>10967833.33333333</v>
+      </c>
+      <c r="Z14">
+        <v>10025750</v>
+      </c>
+      <c r="AA14">
+        <v>9138208.333333332</v>
+      </c>
+      <c r="AB14">
+        <v>8250666.666666666</v>
+      </c>
+      <c r="AC14">
+        <v>7363125</v>
+      </c>
+      <c r="AD14">
+        <v>6490458.333333334</v>
+      </c>
+      <c r="AE14">
+        <v>5617791.666666666</v>
+      </c>
+      <c r="AF14">
+        <v>4745125</v>
+      </c>
+      <c r="AG14">
+        <v>3872458.333333333</v>
+      </c>
+      <c r="AH14">
+        <v>2945250</v>
+      </c>
+      <c r="AI14">
         <v>1963500</v>
       </c>
-      <c r="AI13">
+      <c r="AJ14">
         <v>981750</v>
       </c>
     </row>
@@ -2664,15 +2836,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2776,10 +2948,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -2854,9 +3029,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -2931,9 +3106,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -3008,9 +3183,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -3085,9 +3260,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -3162,9 +3337,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3239,9 +3414,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -3316,9 +3491,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -3393,9 +3568,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -3470,9 +3645,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -3547,9 +3722,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -3624,110 +3799,190 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C13">
+        <v>47</v>
+      </c>
+      <c r="M13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="N13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="O13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="P13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Q13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="R13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="S13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="T13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="U13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="V13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="W13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="X13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Y13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="Z13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AA13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AB13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AC13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AD13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AE13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AF13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AG13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AH13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AI13">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="AJ13">
+        <v>2022976.932083334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C14">
         <v>4045953.864166667</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>6068930.796250001</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>8091907.728333334</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>10114884.66041667</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>12137861.5925</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>14160838.52458333</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>16183815.45666667</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>18206792.38875</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>20229769.32083334</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>22252746.25291667</v>
       </c>
-      <c r="M13">
+      <c r="M14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="N14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="O14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="P14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="Q14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="R14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="S14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="T14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="U14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="V14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="W14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="X14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="Y14">
+        <v>24275723.18500001</v>
+      </c>
+      <c r="Z14">
         <v>22252746.25291667</v>
       </c>
-      <c r="N13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="O13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="P13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="Q13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="R13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="S13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="T13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="U13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="V13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="W13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="X13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="Y13">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="Z13">
+      <c r="AA14">
         <v>20229769.32083334</v>
       </c>
-      <c r="AA13">
+      <c r="AB14">
         <v>18206792.38875</v>
       </c>
-      <c r="AB13">
+      <c r="AC14">
         <v>16183815.45666667</v>
       </c>
-      <c r="AC13">
+      <c r="AD14">
         <v>14160838.52458333</v>
       </c>
-      <c r="AD13">
+      <c r="AE14">
         <v>12137861.5925</v>
       </c>
-      <c r="AE13">
+      <c r="AF14">
         <v>10114884.66041667</v>
       </c>
-      <c r="AF13">
+      <c r="AG14">
         <v>8091907.728333334</v>
       </c>
-      <c r="AG13">
+      <c r="AH14">
         <v>6068930.796250001</v>
       </c>
-      <c r="AH13">
+      <c r="AI14">
         <v>4045953.864166667</v>
       </c>
-      <c r="AI13">
+      <c r="AJ14">
         <v>2022976.932083334</v>
       </c>
     </row>
@@ -3738,15 +3993,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3850,10 +4105,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -3928,9 +4186,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -4005,9 +4263,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -4082,9 +4340,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -4159,9 +4417,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -4236,9 +4494,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -4313,9 +4571,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -4390,9 +4648,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -4467,9 +4725,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -4544,9 +4802,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -4621,9 +4879,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -4698,110 +4956,190 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C13">
+        <v>47</v>
+      </c>
+      <c r="M13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="N13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="O13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="P13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Q13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="R13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="S13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="T13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="U13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="V13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="W13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="X13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Y13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="Z13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AA13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AB13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AC13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AD13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AE13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AF13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AG13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AH13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AI13">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="AJ13">
+        <v>5319315.755833333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C14">
         <v>10638631.51166667</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>15957947.2675</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>21277263.02333333</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>26596578.77916667</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>31915894.535</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>37235210.29083334</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>42554526.04666667</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>47873841.80250001</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>53193157.55833334</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>58512473.31416668</v>
       </c>
-      <c r="M13">
+      <c r="M14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="N14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="O14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="P14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="Q14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="R14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="S14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="T14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="U14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="V14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="W14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="X14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="Y14">
+        <v>63831789.07000002</v>
+      </c>
+      <c r="Z14">
         <v>58512473.31416668</v>
       </c>
-      <c r="N13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="O13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="P13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="Q13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="R13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="S13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="T13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="U13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="V13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="W13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="X13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="Y13">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="Z13">
+      <c r="AA14">
         <v>53193157.55833334</v>
       </c>
-      <c r="AA13">
+      <c r="AB14">
         <v>47873841.80250001</v>
       </c>
-      <c r="AB13">
+      <c r="AC14">
         <v>42554526.04666667</v>
       </c>
-      <c r="AC13">
+      <c r="AD14">
         <v>37235210.29083334</v>
       </c>
-      <c r="AD13">
+      <c r="AE14">
         <v>31915894.535</v>
       </c>
-      <c r="AE13">
+      <c r="AF14">
         <v>26596578.77916667</v>
       </c>
-      <c r="AF13">
+      <c r="AG14">
         <v>21277263.02333333</v>
       </c>
-      <c r="AG13">
+      <c r="AH14">
         <v>15957947.2675</v>
       </c>
-      <c r="AH13">
+      <c r="AI14">
         <v>10638631.51166667</v>
       </c>
-      <c r="AI13">
+      <c r="AJ14">
         <v>5319315.755833333</v>
       </c>
     </row>
@@ -4812,15 +5150,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4924,10 +5262,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -5002,9 +5343,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -5079,9 +5420,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -5156,9 +5497,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -5233,9 +5574,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -5310,9 +5651,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -5387,9 +5728,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -5464,9 +5805,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -5541,9 +5882,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -5618,9 +5959,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -5695,9 +6036,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -5772,110 +6113,190 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C13">
+        <v>47</v>
+      </c>
+      <c r="M13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="N13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="O13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="P13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Q13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="R13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="S13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="T13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="U13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="V13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="W13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="X13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Y13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="Z13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AA13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AB13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AC13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AD13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AE13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AF13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AG13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AH13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AI13">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="AJ13">
+        <v>2833161790.824167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C14">
         <v>5666323581.648334</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>8499485372.4725</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>11332647163.29667</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>14165808954.12083</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>16998970744.945</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>19832132535.76917</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>22665294326.59333</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>25498456117.4175</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>28331617908.24166</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>31164779699.06583</v>
       </c>
-      <c r="M13">
+      <c r="M14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="N14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="O14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="P14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="Q14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="R14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="S14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="T14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="U14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="V14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="W14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="X14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="Y14">
+        <v>33997941489.89</v>
+      </c>
+      <c r="Z14">
         <v>31164779699.06583</v>
       </c>
-      <c r="N13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="O13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="P13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="Q13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="R13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="S13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="T13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="U13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="V13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="W13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="X13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="Y13">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="Z13">
+      <c r="AA14">
         <v>28331617908.24166</v>
       </c>
-      <c r="AA13">
+      <c r="AB14">
         <v>25498456117.4175</v>
       </c>
-      <c r="AB13">
+      <c r="AC14">
         <v>22665294326.59333</v>
       </c>
-      <c r="AC13">
+      <c r="AD14">
         <v>19832132535.76917</v>
       </c>
-      <c r="AD13">
+      <c r="AE14">
         <v>16998970744.945</v>
       </c>
-      <c r="AE13">
+      <c r="AF14">
         <v>14165808954.12083</v>
       </c>
-      <c r="AF13">
+      <c r="AG14">
         <v>11332647163.29667</v>
       </c>
-      <c r="AG13">
+      <c r="AH14">
         <v>8499485372.4725</v>
       </c>
-      <c r="AH13">
+      <c r="AI14">
         <v>5666323581.648334</v>
       </c>
-      <c r="AI13">
+      <c r="AJ14">
         <v>2833161790.824167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2 result in 0910
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="51">
   <si>
     <t>20210618</t>
   </si>
@@ -125,6 +125,9 @@
     <t>20220211</t>
   </si>
   <si>
+    <t>20220218</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -162,6 +165,9 @@
   </si>
   <si>
     <t>20210827-20210903</t>
+  </si>
+  <si>
+    <t>20210903-20210910</t>
   </si>
   <si>
     <t>SUM</t>
@@ -522,15 +528,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -637,10 +643,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -715,9 +724,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -792,9 +801,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -869,9 +878,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -946,9 +955,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1023,9 +1032,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1100,9 +1109,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1177,9 +1186,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1254,9 +1263,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1331,9 +1340,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1408,9 +1417,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1485,9 +1494,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1562,114 +1571,194 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="N14">
+        <v>422993.89125</v>
+      </c>
+      <c r="O14">
+        <v>422993.89125</v>
+      </c>
+      <c r="P14">
+        <v>422993.89125</v>
+      </c>
+      <c r="Q14">
+        <v>422993.89125</v>
+      </c>
+      <c r="R14">
+        <v>422993.89125</v>
+      </c>
+      <c r="S14">
+        <v>422993.89125</v>
+      </c>
+      <c r="T14">
+        <v>422993.89125</v>
+      </c>
+      <c r="U14">
+        <v>422993.89125</v>
+      </c>
+      <c r="V14">
+        <v>422993.89125</v>
+      </c>
+      <c r="W14">
+        <v>422993.89125</v>
+      </c>
+      <c r="X14">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y14">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ14">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK14">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C15">
         <v>1879592.178333333</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>2819388.2675</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>3759184.356666667</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>4801479.284583334</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>5843774.2125</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>6886069.140416667</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>7928364.068333333</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>8765438.304583333</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>9602512.540833334</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>10439586.77708333</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>11276661.01333333</v>
       </c>
-      <c r="N14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="O14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="P14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="Q14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="R14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="S14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="T14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="U14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="V14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="W14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="X14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="Y14">
-        <v>11276661.01333333</v>
-      </c>
-      <c r="Z14">
-        <v>10336864.92416667</v>
-      </c>
-      <c r="AA14">
-        <v>9397068.834999999</v>
-      </c>
-      <c r="AB14">
-        <v>8457272.745833334</v>
-      </c>
-      <c r="AC14">
-        <v>7517476.656666666</v>
-      </c>
-      <c r="AD14">
-        <v>6475181.72875</v>
-      </c>
-      <c r="AE14">
-        <v>5432886.800833333</v>
-      </c>
-      <c r="AF14">
-        <v>4390591.872916667</v>
-      </c>
-      <c r="AG14">
-        <v>3348296.945</v>
-      </c>
-      <c r="AH14">
-        <v>2511222.70875</v>
-      </c>
-      <c r="AI14">
-        <v>1674148.4725</v>
-      </c>
-      <c r="AJ14">
-        <v>837074.2362500001</v>
+      <c r="N15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="O15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="P15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="Q15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="R15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="S15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="T15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="U15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="V15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="W15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="X15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="Y15">
+        <v>11699654.90458333</v>
+      </c>
+      <c r="Z15">
+        <v>10759858.81541667</v>
+      </c>
+      <c r="AA15">
+        <v>9820062.726249998</v>
+      </c>
+      <c r="AB15">
+        <v>8880266.637083333</v>
+      </c>
+      <c r="AC15">
+        <v>7940470.547916667</v>
+      </c>
+      <c r="AD15">
+        <v>6898175.62</v>
+      </c>
+      <c r="AE15">
+        <v>5855880.692083334</v>
+      </c>
+      <c r="AF15">
+        <v>4813585.764166667</v>
+      </c>
+      <c r="AG15">
+        <v>3771290.83625</v>
+      </c>
+      <c r="AH15">
+        <v>2934216.6</v>
+      </c>
+      <c r="AI15">
+        <v>2097142.36375</v>
+      </c>
+      <c r="AJ15">
+        <v>1260068.1275</v>
+      </c>
+      <c r="AK15">
+        <v>422993.89125</v>
       </c>
     </row>
   </sheetData>
@@ -1679,15 +1768,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1794,10 +1883,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -1872,9 +1964,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -1949,9 +2041,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2026,9 +2118,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2103,9 +2195,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2180,9 +2272,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2257,9 +2349,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2334,9 +2426,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2411,9 +2503,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2488,9 +2580,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2565,9 +2657,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -2642,9 +2734,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -2719,114 +2811,194 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
+        <v>49</v>
+      </c>
+      <c r="N14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="O14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="P14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Q14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="R14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="S14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="T14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ14">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK14">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
         <v>942083.3333333334</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>1829625</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>2717166.666666667</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>3604708.333333333</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>4477375</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>5350041.666666667</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>6222708.333333334</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>7095375.000000001</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>8022583.333333334</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>9004333.333333334</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>9986083.333333334</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>10967833.33333333</v>
       </c>
-      <c r="N14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="O14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="P14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="Q14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="R14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="S14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="T14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="U14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="V14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="W14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="X14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="Y14">
-        <v>10967833.33333333</v>
-      </c>
-      <c r="Z14">
-        <v>10025750</v>
-      </c>
-      <c r="AA14">
-        <v>9138208.333333332</v>
-      </c>
-      <c r="AB14">
-        <v>8250666.666666666</v>
-      </c>
-      <c r="AC14">
-        <v>7363125</v>
-      </c>
-      <c r="AD14">
-        <v>6490458.333333334</v>
-      </c>
-      <c r="AE14">
-        <v>5617791.666666666</v>
-      </c>
-      <c r="AF14">
-        <v>4745125</v>
-      </c>
-      <c r="AG14">
-        <v>3872458.333333333</v>
-      </c>
-      <c r="AH14">
-        <v>2945250</v>
-      </c>
-      <c r="AI14">
-        <v>1963500</v>
-      </c>
-      <c r="AJ14">
-        <v>981750</v>
+      <c r="N15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="O15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="P15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="Q15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="R15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="S15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="T15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="U15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="V15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="W15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="X15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="Y15">
+        <v>11669811.42541667</v>
+      </c>
+      <c r="Z15">
+        <v>10727728.09208333</v>
+      </c>
+      <c r="AA15">
+        <v>9840186.425416665</v>
+      </c>
+      <c r="AB15">
+        <v>8952644.758749999</v>
+      </c>
+      <c r="AC15">
+        <v>8065103.092083333</v>
+      </c>
+      <c r="AD15">
+        <v>7192436.425416667</v>
+      </c>
+      <c r="AE15">
+        <v>6319769.758749999</v>
+      </c>
+      <c r="AF15">
+        <v>5447103.092083333</v>
+      </c>
+      <c r="AG15">
+        <v>4574436.425416667</v>
+      </c>
+      <c r="AH15">
+        <v>3647228.092083334</v>
+      </c>
+      <c r="AI15">
+        <v>2665478.092083334</v>
+      </c>
+      <c r="AJ15">
+        <v>1683728.092083334</v>
+      </c>
+      <c r="AK15">
+        <v>701978.0920833334</v>
       </c>
     </row>
   </sheetData>
@@ -2836,15 +3008,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2951,10 +3123,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -3029,9 +3204,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -3106,9 +3281,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -3183,9 +3358,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -3260,9 +3435,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -3337,9 +3512,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3414,9 +3589,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -3491,9 +3666,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -3568,9 +3743,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -3645,9 +3820,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -3722,9 +3897,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -3799,9 +3974,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -3876,114 +4051,194 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="N14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="O14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="P14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Q14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="R14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="S14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="T14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ14">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK14">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C15">
         <v>4045953.864166667</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>6068930.796250001</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>8091907.728333334</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>10114884.66041667</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>12137861.5925</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>14160838.52458333</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>16183815.45666667</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>18206792.38875</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>20229769.32083334</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>22252746.25291667</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>24275723.18500001</v>
       </c>
-      <c r="N14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="O14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="P14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="Q14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="R14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="S14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="T14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="U14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="V14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="W14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="X14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="Y14">
-        <v>24275723.18500001</v>
-      </c>
-      <c r="Z14">
-        <v>22252746.25291667</v>
-      </c>
-      <c r="AA14">
-        <v>20229769.32083334</v>
-      </c>
-      <c r="AB14">
-        <v>18206792.38875</v>
-      </c>
-      <c r="AC14">
-        <v>16183815.45666667</v>
-      </c>
-      <c r="AD14">
-        <v>14160838.52458333</v>
-      </c>
-      <c r="AE14">
-        <v>12137861.5925</v>
-      </c>
-      <c r="AF14">
-        <v>10114884.66041667</v>
-      </c>
-      <c r="AG14">
-        <v>8091907.728333334</v>
-      </c>
-      <c r="AH14">
-        <v>6068930.796250001</v>
-      </c>
-      <c r="AI14">
-        <v>4045953.864166667</v>
-      </c>
-      <c r="AJ14">
-        <v>2022976.932083334</v>
+      <c r="N15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="O15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="P15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="Q15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="R15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="S15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="T15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="U15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="V15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="W15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="X15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="Y15">
+        <v>25788781.48875001</v>
+      </c>
+      <c r="Z15">
+        <v>23765804.55666667</v>
+      </c>
+      <c r="AA15">
+        <v>21742827.62458334</v>
+      </c>
+      <c r="AB15">
+        <v>19719850.6925</v>
+      </c>
+      <c r="AC15">
+        <v>17696873.76041667</v>
+      </c>
+      <c r="AD15">
+        <v>15673896.82833333</v>
+      </c>
+      <c r="AE15">
+        <v>13650919.89625</v>
+      </c>
+      <c r="AF15">
+        <v>11627942.96416667</v>
+      </c>
+      <c r="AG15">
+        <v>9604966.032083334</v>
+      </c>
+      <c r="AH15">
+        <v>7581989.100000001</v>
+      </c>
+      <c r="AI15">
+        <v>5559012.167916667</v>
+      </c>
+      <c r="AJ15">
+        <v>3536035.235833334</v>
+      </c>
+      <c r="AK15">
+        <v>1513058.30375</v>
       </c>
     </row>
   </sheetData>
@@ -3993,15 +4248,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4108,10 +4363,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -4186,9 +4444,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -4263,9 +4521,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -4340,9 +4598,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -4417,9 +4675,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -4494,9 +4752,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -4571,9 +4829,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -4648,9 +4906,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -4725,9 +4983,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -4802,9 +5060,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -4879,9 +5137,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -4956,9 +5214,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -5033,114 +5291,194 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="N14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="O14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="P14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Q14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="R14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="S14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="T14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ14">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK14">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C15">
         <v>10638631.51166667</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>15957947.2675</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>21277263.02333333</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>26596578.77916667</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>31915894.535</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>37235210.29083334</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>42554526.04666667</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>47873841.80250001</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>53193157.55833334</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>58512473.31416668</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>63831789.07000002</v>
       </c>
-      <c r="N14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="O14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="P14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="Q14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="R14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="S14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="T14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="U14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="V14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="W14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="X14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="Y14">
-        <v>63831789.07000002</v>
-      </c>
-      <c r="Z14">
-        <v>58512473.31416668</v>
-      </c>
-      <c r="AA14">
-        <v>53193157.55833334</v>
-      </c>
-      <c r="AB14">
-        <v>47873841.80250001</v>
-      </c>
-      <c r="AC14">
-        <v>42554526.04666667</v>
-      </c>
-      <c r="AD14">
-        <v>37235210.29083334</v>
-      </c>
-      <c r="AE14">
-        <v>31915894.535</v>
-      </c>
-      <c r="AF14">
-        <v>26596578.77916667</v>
-      </c>
-      <c r="AG14">
-        <v>21277263.02333333</v>
-      </c>
-      <c r="AH14">
-        <v>15957947.2675</v>
-      </c>
-      <c r="AI14">
-        <v>10638631.51166667</v>
-      </c>
-      <c r="AJ14">
-        <v>5319315.755833333</v>
+      <c r="N15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="O15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="P15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="Q15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="R15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="S15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="T15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="U15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="V15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="W15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="X15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="Y15">
+        <v>67464492.51208335</v>
+      </c>
+      <c r="Z15">
+        <v>62145176.75625002</v>
+      </c>
+      <c r="AA15">
+        <v>56825861.00041668</v>
+      </c>
+      <c r="AB15">
+        <v>51506545.24458335</v>
+      </c>
+      <c r="AC15">
+        <v>46187229.48875001</v>
+      </c>
+      <c r="AD15">
+        <v>40867913.73291668</v>
+      </c>
+      <c r="AE15">
+        <v>35548597.97708334</v>
+      </c>
+      <c r="AF15">
+        <v>30229282.22125</v>
+      </c>
+      <c r="AG15">
+        <v>24909966.46541667</v>
+      </c>
+      <c r="AH15">
+        <v>19590650.70958333</v>
+      </c>
+      <c r="AI15">
+        <v>14271334.95375</v>
+      </c>
+      <c r="AJ15">
+        <v>8952019.197916666</v>
+      </c>
+      <c r="AK15">
+        <v>3632703.442083333</v>
       </c>
     </row>
   </sheetData>
@@ -5150,15 +5488,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5265,10 +5603,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -5343,9 +5684,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -5420,9 +5761,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -5497,9 +5838,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -5574,9 +5915,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -5651,9 +5992,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -5728,9 +6069,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -5805,9 +6146,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -5882,9 +6223,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -5959,9 +6300,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -6036,9 +6377,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -6113,9 +6454,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -6190,114 +6531,194 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="N14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="O14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="P14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Q14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="R14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="S14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="T14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ14">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK14">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C15">
         <v>5666323581.648334</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>8499485372.4725</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>11332647163.29667</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>14165808954.12083</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>16998970744.945</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>19832132535.76917</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>22665294326.59333</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>25498456117.4175</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>28331617908.24166</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>31164779699.06583</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>33997941489.89</v>
       </c>
-      <c r="N14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="O14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="P14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="Q14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="R14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="S14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="T14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="U14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="V14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="W14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="X14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="Y14">
-        <v>33997941489.89</v>
-      </c>
-      <c r="Z14">
-        <v>31164779699.06583</v>
-      </c>
-      <c r="AA14">
-        <v>28331617908.24166</v>
-      </c>
-      <c r="AB14">
-        <v>25498456117.4175</v>
-      </c>
-      <c r="AC14">
-        <v>22665294326.59333</v>
-      </c>
-      <c r="AD14">
-        <v>19832132535.76917</v>
-      </c>
-      <c r="AE14">
-        <v>16998970744.945</v>
-      </c>
-      <c r="AF14">
-        <v>14165808954.12083</v>
-      </c>
-      <c r="AG14">
-        <v>11332647163.29667</v>
-      </c>
-      <c r="AH14">
-        <v>8499485372.4725</v>
-      </c>
-      <c r="AI14">
-        <v>5666323581.648334</v>
-      </c>
-      <c r="AJ14">
-        <v>2833161790.824167</v>
+      <c r="N15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="O15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="P15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="Q15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="R15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="S15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="T15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="U15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="V15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="W15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="X15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="Y15">
+        <v>36255631271.66458</v>
+      </c>
+      <c r="Z15">
+        <v>33422469480.84041</v>
+      </c>
+      <c r="AA15">
+        <v>30589307690.01625</v>
+      </c>
+      <c r="AB15">
+        <v>27756145899.19208</v>
+      </c>
+      <c r="AC15">
+        <v>24922984108.36792</v>
+      </c>
+      <c r="AD15">
+        <v>22089822317.54375</v>
+      </c>
+      <c r="AE15">
+        <v>19256660526.71959</v>
+      </c>
+      <c r="AF15">
+        <v>16423498735.89542</v>
+      </c>
+      <c r="AG15">
+        <v>13590336945.07125</v>
+      </c>
+      <c r="AH15">
+        <v>10757175154.24708</v>
+      </c>
+      <c r="AI15">
+        <v>7924013363.422916</v>
+      </c>
+      <c r="AJ15">
+        <v>5090851572.59875</v>
+      </c>
+      <c r="AK15">
+        <v>2257689781.774583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2 result in 0917
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="53">
   <si>
     <t>20210618</t>
   </si>
@@ -128,6 +128,9 @@
     <t>20220218</t>
   </si>
   <si>
+    <t>20220225</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -168,6 +171,9 @@
   </si>
   <si>
     <t>20210903-20210910</t>
+  </si>
+  <si>
+    <t>20210910-20210917</t>
   </si>
   <si>
     <t>SUM</t>
@@ -528,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -646,10 +652,13 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -724,9 +733,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -801,9 +810,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -878,9 +887,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -955,9 +964,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1032,9 +1041,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1109,9 +1118,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1186,9 +1195,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1263,9 +1272,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1340,9 +1349,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1417,9 +1426,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1494,9 +1503,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1571,9 +1580,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <v>422993.89125</v>
@@ -1648,116 +1657,196 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>422993.89125</v>
+      </c>
+      <c r="P15">
+        <v>422993.89125</v>
+      </c>
+      <c r="Q15">
+        <v>422993.89125</v>
+      </c>
+      <c r="R15">
+        <v>422993.89125</v>
+      </c>
+      <c r="S15">
+        <v>422993.89125</v>
+      </c>
+      <c r="T15">
+        <v>422993.89125</v>
+      </c>
+      <c r="U15">
+        <v>422993.89125</v>
+      </c>
+      <c r="V15">
+        <v>422993.89125</v>
+      </c>
+      <c r="W15">
+        <v>422993.89125</v>
+      </c>
+      <c r="X15">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y15">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK15">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL15">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C16">
         <v>1879592.178333333</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>2819388.2675</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3759184.356666667</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>4801479.284583334</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>5843774.2125</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>6886069.140416667</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>7928364.068333333</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>8765438.304583333</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>9602512.540833334</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>10439586.77708333</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>11276661.01333333</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>11699654.90458333</v>
       </c>
-      <c r="O15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="P15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="Q15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="R15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="S15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="T15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="U15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="V15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="W15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="X15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="Y15">
-        <v>11699654.90458333</v>
-      </c>
-      <c r="Z15">
-        <v>10759858.81541667</v>
-      </c>
-      <c r="AA15">
-        <v>9820062.726249998</v>
-      </c>
-      <c r="AB15">
-        <v>8880266.637083333</v>
-      </c>
-      <c r="AC15">
-        <v>7940470.547916667</v>
-      </c>
-      <c r="AD15">
-        <v>6898175.62</v>
-      </c>
-      <c r="AE15">
-        <v>5855880.692083334</v>
-      </c>
-      <c r="AF15">
-        <v>4813585.764166667</v>
-      </c>
-      <c r="AG15">
-        <v>3771290.83625</v>
-      </c>
-      <c r="AH15">
-        <v>2934216.6</v>
-      </c>
-      <c r="AI15">
-        <v>2097142.36375</v>
-      </c>
-      <c r="AJ15">
-        <v>1260068.1275</v>
-      </c>
-      <c r="AK15">
+      <c r="O16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="P16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="Q16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="R16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="S16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="T16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="U16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="V16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="W16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="X16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="Y16">
+        <v>12122648.79583333</v>
+      </c>
+      <c r="Z16">
+        <v>11182852.70666667</v>
+      </c>
+      <c r="AA16">
+        <v>10243056.6175</v>
+      </c>
+      <c r="AB16">
+        <v>9303260.528333332</v>
+      </c>
+      <c r="AC16">
+        <v>8363464.439166667</v>
+      </c>
+      <c r="AD16">
+        <v>7321169.51125</v>
+      </c>
+      <c r="AE16">
+        <v>6278874.583333334</v>
+      </c>
+      <c r="AF16">
+        <v>5236579.655416667</v>
+      </c>
+      <c r="AG16">
+        <v>4194284.7275</v>
+      </c>
+      <c r="AH16">
+        <v>3357210.49125</v>
+      </c>
+      <c r="AI16">
+        <v>2520136.255</v>
+      </c>
+      <c r="AJ16">
+        <v>1683062.01875</v>
+      </c>
+      <c r="AK16">
+        <v>845987.7825000001</v>
+      </c>
+      <c r="AL16">
         <v>422993.89125</v>
       </c>
     </row>
@@ -1768,15 +1857,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1886,10 +1975,13 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -1964,9 +2056,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -2041,9 +2133,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2118,9 +2210,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2195,9 +2287,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2272,9 +2364,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2349,9 +2441,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2426,9 +2518,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2503,9 +2595,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2580,9 +2672,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2657,9 +2749,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -2734,9 +2826,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -2811,9 +2903,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <v>701978.0920833334</v>
@@ -2888,116 +2980,196 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="P15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Q15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="R15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="S15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="T15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK15">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL15">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
         <v>942083.3333333334</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>1829625</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>2717166.666666667</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3604708.333333333</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>4477375</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>5350041.666666667</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>6222708.333333334</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>7095375.000000001</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>8022583.333333334</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>9004333.333333334</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>9986083.333333334</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>10967833.33333333</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>11669811.42541667</v>
       </c>
-      <c r="O15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="P15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="Q15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="R15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="S15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="T15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="U15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="V15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="W15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="X15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="Y15">
-        <v>11669811.42541667</v>
-      </c>
-      <c r="Z15">
-        <v>10727728.09208333</v>
-      </c>
-      <c r="AA15">
-        <v>9840186.425416665</v>
-      </c>
-      <c r="AB15">
-        <v>8952644.758749999</v>
-      </c>
-      <c r="AC15">
-        <v>8065103.092083333</v>
-      </c>
-      <c r="AD15">
-        <v>7192436.425416667</v>
-      </c>
-      <c r="AE15">
-        <v>6319769.758749999</v>
-      </c>
-      <c r="AF15">
-        <v>5447103.092083333</v>
-      </c>
-      <c r="AG15">
-        <v>4574436.425416667</v>
-      </c>
-      <c r="AH15">
-        <v>3647228.092083334</v>
-      </c>
-      <c r="AI15">
-        <v>2665478.092083334</v>
-      </c>
-      <c r="AJ15">
-        <v>1683728.092083334</v>
-      </c>
-      <c r="AK15">
+      <c r="O16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="P16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="Q16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="R16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="S16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="T16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="U16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="V16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="W16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="X16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="Y16">
+        <v>12371789.5175</v>
+      </c>
+      <c r="Z16">
+        <v>11429706.18416667</v>
+      </c>
+      <c r="AA16">
+        <v>10542164.5175</v>
+      </c>
+      <c r="AB16">
+        <v>9654622.850833332</v>
+      </c>
+      <c r="AC16">
+        <v>8767081.184166666</v>
+      </c>
+      <c r="AD16">
+        <v>7894414.5175</v>
+      </c>
+      <c r="AE16">
+        <v>7021747.850833332</v>
+      </c>
+      <c r="AF16">
+        <v>6149081.184166666</v>
+      </c>
+      <c r="AG16">
+        <v>5276414.5175</v>
+      </c>
+      <c r="AH16">
+        <v>4349206.184166667</v>
+      </c>
+      <c r="AI16">
+        <v>3367456.184166667</v>
+      </c>
+      <c r="AJ16">
+        <v>2385706.184166667</v>
+      </c>
+      <c r="AK16">
+        <v>1403956.184166667</v>
+      </c>
+      <c r="AL16">
         <v>701978.0920833334</v>
       </c>
     </row>
@@ -3008,15 +3180,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3126,10 +3298,13 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -3204,9 +3379,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -3281,9 +3456,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -3358,9 +3533,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -3435,9 +3610,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -3512,9 +3687,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3589,9 +3764,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -3666,9 +3841,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -3743,9 +3918,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -3820,9 +3995,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -3897,9 +4072,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -3974,9 +4149,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -4051,9 +4226,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <v>1513058.30375</v>
@@ -4128,116 +4303,196 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="P15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Q15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="R15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="S15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="T15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK15">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL15">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C16">
         <v>4045953.864166667</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>6068930.796250001</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>8091907.728333334</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>10114884.66041667</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>12137861.5925</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>14160838.52458333</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>16183815.45666667</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>18206792.38875</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>20229769.32083334</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>22252746.25291667</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>24275723.18500001</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>25788781.48875001</v>
       </c>
-      <c r="O15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="P15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="Q15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="R15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="S15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="T15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="U15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="V15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="W15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="X15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="Y15">
-        <v>25788781.48875001</v>
-      </c>
-      <c r="Z15">
-        <v>23765804.55666667</v>
-      </c>
-      <c r="AA15">
-        <v>21742827.62458334</v>
-      </c>
-      <c r="AB15">
-        <v>19719850.6925</v>
-      </c>
-      <c r="AC15">
-        <v>17696873.76041667</v>
-      </c>
-      <c r="AD15">
-        <v>15673896.82833333</v>
-      </c>
-      <c r="AE15">
-        <v>13650919.89625</v>
-      </c>
-      <c r="AF15">
-        <v>11627942.96416667</v>
-      </c>
-      <c r="AG15">
-        <v>9604966.032083334</v>
-      </c>
-      <c r="AH15">
-        <v>7581989.100000001</v>
-      </c>
-      <c r="AI15">
-        <v>5559012.167916667</v>
-      </c>
-      <c r="AJ15">
-        <v>3536035.235833334</v>
-      </c>
-      <c r="AK15">
+      <c r="O16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="P16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="Q16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="R16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="S16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="T16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="U16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="V16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="W16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="X16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="Y16">
+        <v>27301839.79250001</v>
+      </c>
+      <c r="Z16">
+        <v>25278862.86041667</v>
+      </c>
+      <c r="AA16">
+        <v>23255885.92833334</v>
+      </c>
+      <c r="AB16">
+        <v>21232908.99625</v>
+      </c>
+      <c r="AC16">
+        <v>19209932.06416667</v>
+      </c>
+      <c r="AD16">
+        <v>17186955.13208333</v>
+      </c>
+      <c r="AE16">
+        <v>15163978.2</v>
+      </c>
+      <c r="AF16">
+        <v>13141001.26791667</v>
+      </c>
+      <c r="AG16">
+        <v>11118024.33583333</v>
+      </c>
+      <c r="AH16">
+        <v>9095047.403750001</v>
+      </c>
+      <c r="AI16">
+        <v>7072070.471666667</v>
+      </c>
+      <c r="AJ16">
+        <v>5049093.539583334</v>
+      </c>
+      <c r="AK16">
+        <v>3026116.6075</v>
+      </c>
+      <c r="AL16">
         <v>1513058.30375</v>
       </c>
     </row>
@@ -4248,15 +4503,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4366,10 +4621,13 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -4444,9 +4702,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -4521,9 +4779,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -4598,9 +4856,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -4675,9 +4933,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -4752,9 +5010,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -4829,9 +5087,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -4906,9 +5164,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -4983,9 +5241,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -5060,9 +5318,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -5137,9 +5395,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -5214,9 +5472,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -5291,9 +5549,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <v>3632703.442083333</v>
@@ -5368,116 +5626,196 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="P15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Q15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="R15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="S15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="T15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK15">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL15">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C16">
         <v>10638631.51166667</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>15957947.2675</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>21277263.02333333</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>26596578.77916667</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>31915894.535</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>37235210.29083334</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>42554526.04666667</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>47873841.80250001</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>53193157.55833334</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>58512473.31416668</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>63831789.07000002</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>67464492.51208335</v>
       </c>
-      <c r="O15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="P15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="Q15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="R15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="S15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="T15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="U15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="V15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="W15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="X15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="Y15">
-        <v>67464492.51208335</v>
-      </c>
-      <c r="Z15">
-        <v>62145176.75625002</v>
-      </c>
-      <c r="AA15">
-        <v>56825861.00041668</v>
-      </c>
-      <c r="AB15">
-        <v>51506545.24458335</v>
-      </c>
-      <c r="AC15">
-        <v>46187229.48875001</v>
-      </c>
-      <c r="AD15">
-        <v>40867913.73291668</v>
-      </c>
-      <c r="AE15">
-        <v>35548597.97708334</v>
-      </c>
-      <c r="AF15">
-        <v>30229282.22125</v>
-      </c>
-      <c r="AG15">
-        <v>24909966.46541667</v>
-      </c>
-      <c r="AH15">
-        <v>19590650.70958333</v>
-      </c>
-      <c r="AI15">
-        <v>14271334.95375</v>
-      </c>
-      <c r="AJ15">
-        <v>8952019.197916666</v>
-      </c>
-      <c r="AK15">
+      <c r="O16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="P16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="Q16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="R16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="S16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="T16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="U16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="V16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="W16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="X16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="Y16">
+        <v>71097195.95416668</v>
+      </c>
+      <c r="Z16">
+        <v>65777880.19833335</v>
+      </c>
+      <c r="AA16">
+        <v>60458564.44250002</v>
+      </c>
+      <c r="AB16">
+        <v>55139248.68666668</v>
+      </c>
+      <c r="AC16">
+        <v>49819932.93083335</v>
+      </c>
+      <c r="AD16">
+        <v>44500617.17500001</v>
+      </c>
+      <c r="AE16">
+        <v>39181301.41916668</v>
+      </c>
+      <c r="AF16">
+        <v>33861985.66333333</v>
+      </c>
+      <c r="AG16">
+        <v>28542669.9075</v>
+      </c>
+      <c r="AH16">
+        <v>23223354.15166667</v>
+      </c>
+      <c r="AI16">
+        <v>17904038.39583333</v>
+      </c>
+      <c r="AJ16">
+        <v>12584722.64</v>
+      </c>
+      <c r="AK16">
+        <v>7265406.884166666</v>
+      </c>
+      <c r="AL16">
         <v>3632703.442083333</v>
       </c>
     </row>
@@ -5488,15 +5826,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5606,10 +5944,13 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -5684,9 +6025,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -5761,9 +6102,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -5838,9 +6179,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -5915,9 +6256,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -5992,9 +6333,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -6069,9 +6410,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -6146,9 +6487,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -6223,9 +6564,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -6300,9 +6641,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -6377,9 +6718,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -6454,9 +6795,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -6531,9 +6872,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N14">
         <v>2257689781.774583</v>
@@ -6608,116 +6949,196 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="P15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Q15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="R15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="S15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="T15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK15">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL15">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C16">
         <v>5666323581.648334</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>8499485372.4725</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>11332647163.29667</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>14165808954.12083</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>16998970744.945</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>19832132535.76917</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>22665294326.59333</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>25498456117.4175</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>28331617908.24166</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>31164779699.06583</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>33997941489.89</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>36255631271.66458</v>
       </c>
-      <c r="O15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="P15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="Q15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="R15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="S15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="T15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="U15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="V15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="W15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="X15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="Y15">
-        <v>36255631271.66458</v>
-      </c>
-      <c r="Z15">
-        <v>33422469480.84041</v>
-      </c>
-      <c r="AA15">
-        <v>30589307690.01625</v>
-      </c>
-      <c r="AB15">
-        <v>27756145899.19208</v>
-      </c>
-      <c r="AC15">
-        <v>24922984108.36792</v>
-      </c>
-      <c r="AD15">
-        <v>22089822317.54375</v>
-      </c>
-      <c r="AE15">
-        <v>19256660526.71959</v>
-      </c>
-      <c r="AF15">
-        <v>16423498735.89542</v>
-      </c>
-      <c r="AG15">
-        <v>13590336945.07125</v>
-      </c>
-      <c r="AH15">
-        <v>10757175154.24708</v>
-      </c>
-      <c r="AI15">
-        <v>7924013363.422916</v>
-      </c>
-      <c r="AJ15">
-        <v>5090851572.59875</v>
-      </c>
-      <c r="AK15">
+      <c r="O16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="P16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="Q16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="R16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="S16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="T16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="U16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="V16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="W16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="X16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="Y16">
+        <v>38513321053.43916</v>
+      </c>
+      <c r="Z16">
+        <v>35680159262.615</v>
+      </c>
+      <c r="AA16">
+        <v>32846997471.79083</v>
+      </c>
+      <c r="AB16">
+        <v>30013835680.96666</v>
+      </c>
+      <c r="AC16">
+        <v>27180673890.1425</v>
+      </c>
+      <c r="AD16">
+        <v>24347512099.31833</v>
+      </c>
+      <c r="AE16">
+        <v>21514350308.49417</v>
+      </c>
+      <c r="AF16">
+        <v>18681188517.67</v>
+      </c>
+      <c r="AG16">
+        <v>15848026726.84583</v>
+      </c>
+      <c r="AH16">
+        <v>13014864936.02167</v>
+      </c>
+      <c r="AI16">
+        <v>10181703145.1975</v>
+      </c>
+      <c r="AJ16">
+        <v>7348541354.373333</v>
+      </c>
+      <c r="AK16">
+        <v>4515379563.549167</v>
+      </c>
+      <c r="AL16">
         <v>2257689781.774583</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2 result in 0924
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="55">
   <si>
     <t>20210618</t>
   </si>
@@ -131,6 +131,9 @@
     <t>20220225</t>
   </si>
   <si>
+    <t>20220304</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -174,6 +177,9 @@
   </si>
   <si>
     <t>20210910-20210917</t>
+  </si>
+  <si>
+    <t>20210917-20210924</t>
   </si>
   <si>
     <t>SUM</t>
@@ -534,15 +540,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -655,10 +661,13 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -733,9 +742,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -810,9 +819,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -887,9 +896,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -964,9 +973,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1041,9 +1050,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1118,9 +1127,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1195,9 +1204,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1272,9 +1281,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1349,9 +1358,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1426,9 +1435,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1503,9 +1512,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1580,9 +1589,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:39">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>422993.89125</v>
@@ -1657,9 +1666,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:39">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O15">
         <v>422993.89125</v>
@@ -1734,119 +1743,199 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:39">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C16">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>422993.89125</v>
+      </c>
+      <c r="Q16">
+        <v>422993.89125</v>
+      </c>
+      <c r="R16">
+        <v>422993.89125</v>
+      </c>
+      <c r="S16">
+        <v>422993.89125</v>
+      </c>
+      <c r="T16">
+        <v>422993.89125</v>
+      </c>
+      <c r="U16">
+        <v>422993.89125</v>
+      </c>
+      <c r="V16">
+        <v>422993.89125</v>
+      </c>
+      <c r="W16">
+        <v>422993.89125</v>
+      </c>
+      <c r="X16">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y16">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL16">
+        <v>422993.89125</v>
+      </c>
+      <c r="AM16">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C17">
         <v>1879592.178333333</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>2819388.2675</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>3759184.356666667</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>4801479.284583334</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>5843774.2125</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>6886069.140416667</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>7928364.068333333</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>8765438.304583333</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>9602512.540833334</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>10439586.77708333</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>11276661.01333333</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>11699654.90458333</v>
       </c>
-      <c r="O16">
+      <c r="O17">
         <v>12122648.79583333</v>
       </c>
-      <c r="P16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="Q16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="R16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="S16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="T16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="U16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="V16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="W16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="X16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="Y16">
-        <v>12122648.79583333</v>
-      </c>
-      <c r="Z16">
-        <v>11182852.70666667</v>
-      </c>
-      <c r="AA16">
-        <v>10243056.6175</v>
-      </c>
-      <c r="AB16">
-        <v>9303260.528333332</v>
-      </c>
-      <c r="AC16">
-        <v>8363464.439166667</v>
-      </c>
-      <c r="AD16">
-        <v>7321169.51125</v>
-      </c>
-      <c r="AE16">
-        <v>6278874.583333334</v>
-      </c>
-      <c r="AF16">
-        <v>5236579.655416667</v>
-      </c>
-      <c r="AG16">
-        <v>4194284.7275</v>
-      </c>
-      <c r="AH16">
-        <v>3357210.49125</v>
-      </c>
-      <c r="AI16">
-        <v>2520136.255</v>
-      </c>
-      <c r="AJ16">
-        <v>1683062.01875</v>
-      </c>
-      <c r="AK16">
+      <c r="P17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="Q17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="R17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="S17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="T17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="U17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="V17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="W17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="X17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="Y17">
+        <v>12545642.68708333</v>
+      </c>
+      <c r="Z17">
+        <v>11605846.59791666</v>
+      </c>
+      <c r="AA17">
+        <v>10666050.50875</v>
+      </c>
+      <c r="AB17">
+        <v>9726254.419583332</v>
+      </c>
+      <c r="AC17">
+        <v>8786458.330416666</v>
+      </c>
+      <c r="AD17">
+        <v>7744163.402500001</v>
+      </c>
+      <c r="AE17">
+        <v>6701868.474583334</v>
+      </c>
+      <c r="AF17">
+        <v>5659573.546666668</v>
+      </c>
+      <c r="AG17">
+        <v>4617278.61875</v>
+      </c>
+      <c r="AH17">
+        <v>3780204.3825</v>
+      </c>
+      <c r="AI17">
+        <v>2943130.14625</v>
+      </c>
+      <c r="AJ17">
+        <v>2106055.91</v>
+      </c>
+      <c r="AK17">
+        <v>1268981.67375</v>
+      </c>
+      <c r="AL17">
         <v>845987.7825000001</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>422993.89125</v>
       </c>
     </row>
@@ -1857,15 +1946,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1978,10 +2067,13 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -2056,9 +2148,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -2133,9 +2225,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2210,9 +2302,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2287,9 +2379,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2364,9 +2456,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2441,9 +2533,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2518,9 +2610,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2595,9 +2687,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2672,9 +2764,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2749,9 +2841,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -2826,9 +2918,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -2903,9 +2995,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:39">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>701978.0920833334</v>
@@ -2980,9 +3072,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:39">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O15">
         <v>701978.0920833334</v>
@@ -3057,119 +3149,199 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:39">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Q16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="R16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="S16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="T16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL16">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AM16">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
         <v>942083.3333333334</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>1829625</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>2717166.666666667</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>3604708.333333333</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>4477375</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>5350041.666666667</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>6222708.333333334</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>7095375.000000001</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>8022583.333333334</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>9004333.333333334</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>9986083.333333334</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>10967833.33333333</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>11669811.42541667</v>
       </c>
-      <c r="O16">
+      <c r="O17">
         <v>12371789.5175</v>
       </c>
-      <c r="P16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="Q16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="R16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="S16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="T16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="U16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="V16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="W16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="X16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="Y16">
-        <v>12371789.5175</v>
-      </c>
-      <c r="Z16">
-        <v>11429706.18416667</v>
-      </c>
-      <c r="AA16">
-        <v>10542164.5175</v>
-      </c>
-      <c r="AB16">
-        <v>9654622.850833332</v>
-      </c>
-      <c r="AC16">
-        <v>8767081.184166666</v>
-      </c>
-      <c r="AD16">
-        <v>7894414.5175</v>
-      </c>
-      <c r="AE16">
-        <v>7021747.850833332</v>
-      </c>
-      <c r="AF16">
-        <v>6149081.184166666</v>
-      </c>
-      <c r="AG16">
-        <v>5276414.5175</v>
-      </c>
-      <c r="AH16">
-        <v>4349206.184166667</v>
-      </c>
-      <c r="AI16">
-        <v>3367456.184166667</v>
-      </c>
-      <c r="AJ16">
-        <v>2385706.184166667</v>
-      </c>
-      <c r="AK16">
+      <c r="P17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="Q17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="R17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="S17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="T17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="U17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="V17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="W17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="X17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="Y17">
+        <v>13073767.60958333</v>
+      </c>
+      <c r="Z17">
+        <v>12131684.27625</v>
+      </c>
+      <c r="AA17">
+        <v>11244142.60958333</v>
+      </c>
+      <c r="AB17">
+        <v>10356600.94291667</v>
+      </c>
+      <c r="AC17">
+        <v>9469059.276249999</v>
+      </c>
+      <c r="AD17">
+        <v>8596392.609583333</v>
+      </c>
+      <c r="AE17">
+        <v>7723725.942916665</v>
+      </c>
+      <c r="AF17">
+        <v>6851059.276249999</v>
+      </c>
+      <c r="AG17">
+        <v>5978392.609583333</v>
+      </c>
+      <c r="AH17">
+        <v>5051184.27625</v>
+      </c>
+      <c r="AI17">
+        <v>4069434.276250001</v>
+      </c>
+      <c r="AJ17">
+        <v>3087684.276250001</v>
+      </c>
+      <c r="AK17">
+        <v>2105934.27625</v>
+      </c>
+      <c r="AL17">
         <v>1403956.184166667</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>701978.0920833334</v>
       </c>
     </row>
@@ -3180,15 +3352,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3301,10 +3473,13 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -3379,9 +3554,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -3456,9 +3631,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -3533,9 +3708,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -3610,9 +3785,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -3687,9 +3862,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3764,9 +3939,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -3841,9 +4016,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -3918,9 +4093,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -3995,9 +4170,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -4072,9 +4247,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -4149,9 +4324,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -4226,9 +4401,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:39">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>1513058.30375</v>
@@ -4303,9 +4478,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:39">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O15">
         <v>1513058.30375</v>
@@ -4380,119 +4555,199 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:39">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C16">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Q16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="R16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="S16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="T16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL16">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AM16">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C17">
         <v>4045953.864166667</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>6068930.796250001</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>8091907.728333334</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>10114884.66041667</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>12137861.5925</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>14160838.52458333</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>16183815.45666667</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>18206792.38875</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>20229769.32083334</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>22252746.25291667</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>24275723.18500001</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>25788781.48875001</v>
       </c>
-      <c r="O16">
+      <c r="O17">
         <v>27301839.79250001</v>
       </c>
-      <c r="P16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="Q16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="R16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="S16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="T16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="U16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="V16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="W16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="X16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="Y16">
-        <v>27301839.79250001</v>
-      </c>
-      <c r="Z16">
-        <v>25278862.86041667</v>
-      </c>
-      <c r="AA16">
-        <v>23255885.92833334</v>
-      </c>
-      <c r="AB16">
-        <v>21232908.99625</v>
-      </c>
-      <c r="AC16">
-        <v>19209932.06416667</v>
-      </c>
-      <c r="AD16">
-        <v>17186955.13208333</v>
-      </c>
-      <c r="AE16">
-        <v>15163978.2</v>
-      </c>
-      <c r="AF16">
-        <v>13141001.26791667</v>
-      </c>
-      <c r="AG16">
-        <v>11118024.33583333</v>
-      </c>
-      <c r="AH16">
-        <v>9095047.403750001</v>
-      </c>
-      <c r="AI16">
-        <v>7072070.471666667</v>
-      </c>
-      <c r="AJ16">
-        <v>5049093.539583334</v>
-      </c>
-      <c r="AK16">
+      <c r="P17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="Q17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="R17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="S17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="T17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="U17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="V17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="W17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="X17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="Y17">
+        <v>28814898.09625001</v>
+      </c>
+      <c r="Z17">
+        <v>26791921.16416667</v>
+      </c>
+      <c r="AA17">
+        <v>24768944.23208334</v>
+      </c>
+      <c r="AB17">
+        <v>22745967.3</v>
+      </c>
+      <c r="AC17">
+        <v>20722990.36791667</v>
+      </c>
+      <c r="AD17">
+        <v>18700013.43583333</v>
+      </c>
+      <c r="AE17">
+        <v>16677036.50375</v>
+      </c>
+      <c r="AF17">
+        <v>14654059.57166667</v>
+      </c>
+      <c r="AG17">
+        <v>12631082.63958333</v>
+      </c>
+      <c r="AH17">
+        <v>10608105.7075</v>
+      </c>
+      <c r="AI17">
+        <v>8585128.775416667</v>
+      </c>
+      <c r="AJ17">
+        <v>6562151.843333334</v>
+      </c>
+      <c r="AK17">
+        <v>4539174.91125</v>
+      </c>
+      <c r="AL17">
         <v>3026116.6075</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>1513058.30375</v>
       </c>
     </row>
@@ -4503,15 +4758,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4624,10 +4879,13 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -4702,9 +4960,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -4779,9 +5037,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -4856,9 +5114,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -4933,9 +5191,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -5010,9 +5268,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -5087,9 +5345,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -5164,9 +5422,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -5241,9 +5499,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -5318,9 +5576,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -5395,9 +5653,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -5472,9 +5730,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -5549,9 +5807,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:39">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>3632703.442083333</v>
@@ -5626,9 +5884,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:39">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O15">
         <v>3632703.442083333</v>
@@ -5703,119 +5961,199 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:39">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C16">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Q16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="R16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="S16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="T16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL16">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AM16">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C17">
         <v>10638631.51166667</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>15957947.2675</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>21277263.02333333</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>26596578.77916667</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>31915894.535</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>37235210.29083334</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>42554526.04666667</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>47873841.80250001</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>53193157.55833334</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>58512473.31416668</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>63831789.07000002</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>67464492.51208335</v>
       </c>
-      <c r="O16">
+      <c r="O17">
         <v>71097195.95416668</v>
       </c>
-      <c r="P16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="Q16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="R16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="S16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="T16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="U16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="V16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="W16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="X16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="Y16">
-        <v>71097195.95416668</v>
-      </c>
-      <c r="Z16">
-        <v>65777880.19833335</v>
-      </c>
-      <c r="AA16">
-        <v>60458564.44250002</v>
-      </c>
-      <c r="AB16">
-        <v>55139248.68666668</v>
-      </c>
-      <c r="AC16">
-        <v>49819932.93083335</v>
-      </c>
-      <c r="AD16">
-        <v>44500617.17500001</v>
-      </c>
-      <c r="AE16">
-        <v>39181301.41916668</v>
-      </c>
-      <c r="AF16">
-        <v>33861985.66333333</v>
-      </c>
-      <c r="AG16">
-        <v>28542669.9075</v>
-      </c>
-      <c r="AH16">
-        <v>23223354.15166667</v>
-      </c>
-      <c r="AI16">
-        <v>17904038.39583333</v>
-      </c>
-      <c r="AJ16">
-        <v>12584722.64</v>
-      </c>
-      <c r="AK16">
+      <c r="P17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="Q17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="R17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="S17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="T17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="U17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="V17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="W17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="X17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="Y17">
+        <v>74729899.39625001</v>
+      </c>
+      <c r="Z17">
+        <v>69410583.64041668</v>
+      </c>
+      <c r="AA17">
+        <v>64091267.88458335</v>
+      </c>
+      <c r="AB17">
+        <v>58771952.12875002</v>
+      </c>
+      <c r="AC17">
+        <v>53452636.37291668</v>
+      </c>
+      <c r="AD17">
+        <v>48133320.61708335</v>
+      </c>
+      <c r="AE17">
+        <v>42814004.86125001</v>
+      </c>
+      <c r="AF17">
+        <v>37494689.10541667</v>
+      </c>
+      <c r="AG17">
+        <v>32175373.34958333</v>
+      </c>
+      <c r="AH17">
+        <v>26856057.59375</v>
+      </c>
+      <c r="AI17">
+        <v>21536741.83791666</v>
+      </c>
+      <c r="AJ17">
+        <v>16217426.08208333</v>
+      </c>
+      <c r="AK17">
+        <v>10898110.32625</v>
+      </c>
+      <c r="AL17">
         <v>7265406.884166666</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>3632703.442083333</v>
       </c>
     </row>
@@ -5826,15 +6164,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5947,10 +6285,13 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -6025,9 +6366,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -6102,9 +6443,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -6179,9 +6520,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -6256,9 +6597,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -6333,9 +6674,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -6410,9 +6751,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -6487,9 +6828,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -6564,9 +6905,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -6641,9 +6982,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -6718,9 +7059,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -6795,9 +7136,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -6872,9 +7213,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:39">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>2257689781.774583</v>
@@ -6949,9 +7290,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:39">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O15">
         <v>2257689781.774583</v>
@@ -7026,119 +7367,199 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:39">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C16">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Q16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="R16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="S16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="T16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL16">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AM16">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C17">
         <v>5666323581.648334</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>8499485372.4725</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>11332647163.29667</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>14165808954.12083</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>16998970744.945</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>19832132535.76917</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>22665294326.59333</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>25498456117.4175</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>28331617908.24166</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>31164779699.06583</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>33997941489.89</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>36255631271.66458</v>
       </c>
-      <c r="O16">
+      <c r="O17">
         <v>38513321053.43916</v>
       </c>
-      <c r="P16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="Q16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="R16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="S16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="T16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="U16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="V16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="W16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="X16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="Y16">
-        <v>38513321053.43916</v>
-      </c>
-      <c r="Z16">
-        <v>35680159262.615</v>
-      </c>
-      <c r="AA16">
-        <v>32846997471.79083</v>
-      </c>
-      <c r="AB16">
-        <v>30013835680.96666</v>
-      </c>
-      <c r="AC16">
-        <v>27180673890.1425</v>
-      </c>
-      <c r="AD16">
-        <v>24347512099.31833</v>
-      </c>
-      <c r="AE16">
-        <v>21514350308.49417</v>
-      </c>
-      <c r="AF16">
-        <v>18681188517.67</v>
-      </c>
-      <c r="AG16">
-        <v>15848026726.84583</v>
-      </c>
-      <c r="AH16">
-        <v>13014864936.02167</v>
-      </c>
-      <c r="AI16">
-        <v>10181703145.1975</v>
-      </c>
-      <c r="AJ16">
-        <v>7348541354.373333</v>
-      </c>
-      <c r="AK16">
+      <c r="P17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="Q17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="R17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="S17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="T17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="U17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="V17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="W17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="X17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="Y17">
+        <v>40771010835.21375</v>
+      </c>
+      <c r="Z17">
+        <v>37937849044.38958</v>
+      </c>
+      <c r="AA17">
+        <v>35104687253.56541</v>
+      </c>
+      <c r="AB17">
+        <v>32271525462.74125</v>
+      </c>
+      <c r="AC17">
+        <v>29438363671.91708</v>
+      </c>
+      <c r="AD17">
+        <v>26605201881.09291</v>
+      </c>
+      <c r="AE17">
+        <v>23772040090.26875</v>
+      </c>
+      <c r="AF17">
+        <v>20938878299.44458</v>
+      </c>
+      <c r="AG17">
+        <v>18105716508.62042</v>
+      </c>
+      <c r="AH17">
+        <v>15272554717.79625</v>
+      </c>
+      <c r="AI17">
+        <v>12439392926.97208</v>
+      </c>
+      <c r="AJ17">
+        <v>9606231136.147917</v>
+      </c>
+      <c r="AK17">
+        <v>6773069345.32375</v>
+      </c>
+      <c r="AL17">
         <v>4515379563.549167</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>2257689781.774583</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2 result in 1001
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="57">
   <si>
     <t>20210618</t>
   </si>
@@ -134,6 +134,9 @@
     <t>20220304</t>
   </si>
   <si>
+    <t>20220311</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -180,6 +183,9 @@
   </si>
   <si>
     <t>20210917-20210924</t>
+  </si>
+  <si>
+    <t>20210924-20211001</t>
   </si>
   <si>
     <t>SUM</t>
@@ -540,15 +546,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -664,10 +670,13 @@
       <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -742,9 +751,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -819,9 +828,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -896,9 +905,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -973,9 +982,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1050,9 +1059,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1127,9 +1136,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1204,9 +1213,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1281,9 +1290,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1358,9 +1367,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1435,9 +1444,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1512,9 +1521,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1589,9 +1598,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14">
         <v>422993.89125</v>
@@ -1666,9 +1675,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:40">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O15">
         <v>422993.89125</v>
@@ -1743,9 +1752,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P16">
         <v>422993.89125</v>
@@ -1820,122 +1829,202 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:40">
       <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="Q17">
+        <v>422993.89125</v>
+      </c>
+      <c r="R17">
+        <v>422993.89125</v>
+      </c>
+      <c r="S17">
+        <v>422993.89125</v>
+      </c>
+      <c r="T17">
+        <v>422993.89125</v>
+      </c>
+      <c r="U17">
+        <v>422993.89125</v>
+      </c>
+      <c r="V17">
+        <v>422993.89125</v>
+      </c>
+      <c r="W17">
+        <v>422993.89125</v>
+      </c>
+      <c r="X17">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y17">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AM17">
+        <v>422993.89125</v>
+      </c>
+      <c r="AN17">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C18">
         <v>1879592.178333333</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>2819388.2675</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>3759184.356666667</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>4801479.284583334</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>5843774.2125</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>6886069.140416667</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>7928364.068333333</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>8765438.304583333</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>9602512.540833334</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>10439586.77708333</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>11276661.01333333</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>11699654.90458333</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>12122648.79583333</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>12545642.68708333</v>
       </c>
-      <c r="Q17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="R17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="S17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="T17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="U17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="V17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="W17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="X17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="Y17">
-        <v>12545642.68708333</v>
-      </c>
-      <c r="Z17">
-        <v>11605846.59791666</v>
-      </c>
-      <c r="AA17">
-        <v>10666050.50875</v>
-      </c>
-      <c r="AB17">
-        <v>9726254.419583332</v>
-      </c>
-      <c r="AC17">
-        <v>8786458.330416666</v>
-      </c>
-      <c r="AD17">
-        <v>7744163.402500001</v>
-      </c>
-      <c r="AE17">
-        <v>6701868.474583334</v>
-      </c>
-      <c r="AF17">
-        <v>5659573.546666668</v>
-      </c>
-      <c r="AG17">
-        <v>4617278.61875</v>
-      </c>
-      <c r="AH17">
-        <v>3780204.3825</v>
-      </c>
-      <c r="AI17">
-        <v>2943130.14625</v>
-      </c>
-      <c r="AJ17">
-        <v>2106055.91</v>
-      </c>
-      <c r="AK17">
+      <c r="Q18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="R18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="S18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="T18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="U18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="V18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="W18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="X18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="Y18">
+        <v>12968636.57833333</v>
+      </c>
+      <c r="Z18">
+        <v>12028840.48916666</v>
+      </c>
+      <c r="AA18">
+        <v>11089044.4</v>
+      </c>
+      <c r="AB18">
+        <v>10149248.31083333</v>
+      </c>
+      <c r="AC18">
+        <v>9209452.221666666</v>
+      </c>
+      <c r="AD18">
+        <v>8167157.293750001</v>
+      </c>
+      <c r="AE18">
+        <v>7124862.365833335</v>
+      </c>
+      <c r="AF18">
+        <v>6082567.437916668</v>
+      </c>
+      <c r="AG18">
+        <v>5040272.510000001</v>
+      </c>
+      <c r="AH18">
+        <v>4203198.27375</v>
+      </c>
+      <c r="AI18">
+        <v>3366124.0375</v>
+      </c>
+      <c r="AJ18">
+        <v>2529049.80125</v>
+      </c>
+      <c r="AK18">
+        <v>1691975.565</v>
+      </c>
+      <c r="AL18">
         <v>1268981.67375</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>845987.7825000001</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>422993.89125</v>
       </c>
     </row>
@@ -1946,15 +2035,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2070,10 +2159,13 @@
       <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -2148,9 +2240,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -2225,9 +2317,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2302,9 +2394,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2379,9 +2471,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2456,9 +2548,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2533,9 +2625,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2610,9 +2702,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2687,9 +2779,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2764,9 +2856,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -2841,9 +2933,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -2918,9 +3010,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -2995,9 +3087,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14">
         <v>701978.0920833334</v>
@@ -3072,9 +3164,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:40">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O15">
         <v>701978.0920833334</v>
@@ -3149,9 +3241,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P16">
         <v>701978.0920833334</v>
@@ -3226,122 +3318,202 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:40">
       <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
+        <v>55</v>
+      </c>
+      <c r="Q17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="R17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="S17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="T17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AM17">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AN17">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
         <v>942083.3333333334</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1829625</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>2717166.666666667</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>3604708.333333333</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>4477375</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>5350041.666666667</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>6222708.333333334</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>7095375.000000001</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>8022583.333333334</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>9004333.333333334</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>9986083.333333334</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>10967833.33333333</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>11669811.42541667</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>12371789.5175</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>13073767.60958333</v>
       </c>
-      <c r="Q17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="R17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="S17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="T17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="U17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="V17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="W17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="X17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="Y17">
-        <v>13073767.60958333</v>
-      </c>
-      <c r="Z17">
-        <v>12131684.27625</v>
-      </c>
-      <c r="AA17">
-        <v>11244142.60958333</v>
-      </c>
-      <c r="AB17">
-        <v>10356600.94291667</v>
-      </c>
-      <c r="AC17">
-        <v>9469059.276249999</v>
-      </c>
-      <c r="AD17">
-        <v>8596392.609583333</v>
-      </c>
-      <c r="AE17">
-        <v>7723725.942916665</v>
-      </c>
-      <c r="AF17">
-        <v>6851059.276249999</v>
-      </c>
-      <c r="AG17">
-        <v>5978392.609583333</v>
-      </c>
-      <c r="AH17">
-        <v>5051184.27625</v>
-      </c>
-      <c r="AI17">
-        <v>4069434.276250001</v>
-      </c>
-      <c r="AJ17">
-        <v>3087684.276250001</v>
-      </c>
-      <c r="AK17">
+      <c r="Q18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="R18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="S18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="T18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="U18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="V18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="W18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="X18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="Y18">
+        <v>13775745.70166667</v>
+      </c>
+      <c r="Z18">
+        <v>12833662.36833333</v>
+      </c>
+      <c r="AA18">
+        <v>11946120.70166666</v>
+      </c>
+      <c r="AB18">
+        <v>11058579.035</v>
+      </c>
+      <c r="AC18">
+        <v>10171037.36833333</v>
+      </c>
+      <c r="AD18">
+        <v>9298370.701666666</v>
+      </c>
+      <c r="AE18">
+        <v>8425704.034999998</v>
+      </c>
+      <c r="AF18">
+        <v>7553037.368333332</v>
+      </c>
+      <c r="AG18">
+        <v>6680370.701666666</v>
+      </c>
+      <c r="AH18">
+        <v>5753162.368333333</v>
+      </c>
+      <c r="AI18">
+        <v>4771412.368333334</v>
+      </c>
+      <c r="AJ18">
+        <v>3789662.368333334</v>
+      </c>
+      <c r="AK18">
+        <v>2807912.368333334</v>
+      </c>
+      <c r="AL18">
         <v>2105934.27625</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>1403956.184166667</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>701978.0920833334</v>
       </c>
     </row>
@@ -3352,15 +3524,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3476,10 +3648,13 @@
       <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -3554,9 +3729,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -3631,9 +3806,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -3708,9 +3883,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -3785,9 +3960,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -3862,9 +4037,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -3939,9 +4114,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -4016,9 +4191,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -4093,9 +4268,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -4170,9 +4345,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -4247,9 +4422,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -4324,9 +4499,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -4401,9 +4576,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14">
         <v>1513058.30375</v>
@@ -4478,9 +4653,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:40">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O15">
         <v>1513058.30375</v>
@@ -4555,9 +4730,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P16">
         <v>1513058.30375</v>
@@ -4632,122 +4807,202 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:40">
       <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="Q17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="R17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="S17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="T17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AM17">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AN17">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C18">
         <v>4045953.864166667</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>6068930.796250001</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>8091907.728333334</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>10114884.66041667</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>12137861.5925</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>14160838.52458333</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>16183815.45666667</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>18206792.38875</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>20229769.32083334</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>22252746.25291667</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>24275723.18500001</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>25788781.48875001</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>27301839.79250001</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>28814898.09625001</v>
       </c>
-      <c r="Q17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="R17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="S17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="T17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="U17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="V17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="W17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="X17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="Y17">
-        <v>28814898.09625001</v>
-      </c>
-      <c r="Z17">
-        <v>26791921.16416667</v>
-      </c>
-      <c r="AA17">
-        <v>24768944.23208334</v>
-      </c>
-      <c r="AB17">
-        <v>22745967.3</v>
-      </c>
-      <c r="AC17">
-        <v>20722990.36791667</v>
-      </c>
-      <c r="AD17">
-        <v>18700013.43583333</v>
-      </c>
-      <c r="AE17">
-        <v>16677036.50375</v>
-      </c>
-      <c r="AF17">
-        <v>14654059.57166667</v>
-      </c>
-      <c r="AG17">
-        <v>12631082.63958333</v>
-      </c>
-      <c r="AH17">
-        <v>10608105.7075</v>
-      </c>
-      <c r="AI17">
-        <v>8585128.775416667</v>
-      </c>
-      <c r="AJ17">
-        <v>6562151.843333334</v>
-      </c>
-      <c r="AK17">
+      <c r="Q18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="R18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="S18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="T18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="U18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="V18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="W18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="X18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="Y18">
+        <v>30327956.40000001</v>
+      </c>
+      <c r="Z18">
+        <v>28304979.46791667</v>
+      </c>
+      <c r="AA18">
+        <v>26282002.53583334</v>
+      </c>
+      <c r="AB18">
+        <v>24259025.60375001</v>
+      </c>
+      <c r="AC18">
+        <v>22236048.67166667</v>
+      </c>
+      <c r="AD18">
+        <v>20213071.73958334</v>
+      </c>
+      <c r="AE18">
+        <v>18190094.8075</v>
+      </c>
+      <c r="AF18">
+        <v>16167117.87541667</v>
+      </c>
+      <c r="AG18">
+        <v>14144140.94333334</v>
+      </c>
+      <c r="AH18">
+        <v>12121164.01125</v>
+      </c>
+      <c r="AI18">
+        <v>10098187.07916667</v>
+      </c>
+      <c r="AJ18">
+        <v>8075210.147083334</v>
+      </c>
+      <c r="AK18">
+        <v>6052233.215</v>
+      </c>
+      <c r="AL18">
         <v>4539174.91125</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>3026116.6075</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>1513058.30375</v>
       </c>
     </row>
@@ -4758,15 +5013,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4882,10 +5137,13 @@
       <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -4960,9 +5218,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -5037,9 +5295,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -5114,9 +5372,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -5191,9 +5449,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -5268,9 +5526,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -5345,9 +5603,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -5422,9 +5680,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -5499,9 +5757,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -5576,9 +5834,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -5653,9 +5911,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -5730,9 +5988,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -5807,9 +6065,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14">
         <v>3632703.442083333</v>
@@ -5884,9 +6142,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:40">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O15">
         <v>3632703.442083333</v>
@@ -5961,9 +6219,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P16">
         <v>3632703.442083333</v>
@@ -6038,122 +6296,202 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:40">
       <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="Q17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="R17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="S17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="T17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AM17">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AN17">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C18">
         <v>10638631.51166667</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>15957947.2675</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>21277263.02333333</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>26596578.77916667</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>31915894.535</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>37235210.29083334</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>42554526.04666667</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>47873841.80250001</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>53193157.55833334</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>58512473.31416668</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>63831789.07000002</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>67464492.51208335</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>71097195.95416668</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>74729899.39625001</v>
       </c>
-      <c r="Q17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="R17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="S17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="T17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="U17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="V17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="W17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="X17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="Y17">
-        <v>74729899.39625001</v>
-      </c>
-      <c r="Z17">
-        <v>69410583.64041668</v>
-      </c>
-      <c r="AA17">
-        <v>64091267.88458335</v>
-      </c>
-      <c r="AB17">
-        <v>58771952.12875002</v>
-      </c>
-      <c r="AC17">
-        <v>53452636.37291668</v>
-      </c>
-      <c r="AD17">
-        <v>48133320.61708335</v>
-      </c>
-      <c r="AE17">
-        <v>42814004.86125001</v>
-      </c>
-      <c r="AF17">
-        <v>37494689.10541667</v>
-      </c>
-      <c r="AG17">
-        <v>32175373.34958333</v>
-      </c>
-      <c r="AH17">
-        <v>26856057.59375</v>
-      </c>
-      <c r="AI17">
-        <v>21536741.83791666</v>
-      </c>
-      <c r="AJ17">
-        <v>16217426.08208333</v>
-      </c>
-      <c r="AK17">
+      <c r="Q18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="R18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="S18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="T18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="U18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="V18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="W18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="X18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="Y18">
+        <v>78362602.83833334</v>
+      </c>
+      <c r="Z18">
+        <v>73043287.08250001</v>
+      </c>
+      <c r="AA18">
+        <v>67723971.32666668</v>
+      </c>
+      <c r="AB18">
+        <v>62404655.57083336</v>
+      </c>
+      <c r="AC18">
+        <v>57085339.81500002</v>
+      </c>
+      <c r="AD18">
+        <v>51766024.05916668</v>
+      </c>
+      <c r="AE18">
+        <v>46446708.30333335</v>
+      </c>
+      <c r="AF18">
+        <v>41127392.54750001</v>
+      </c>
+      <c r="AG18">
+        <v>35808076.79166666</v>
+      </c>
+      <c r="AH18">
+        <v>30488761.03583333</v>
+      </c>
+      <c r="AI18">
+        <v>25169445.28</v>
+      </c>
+      <c r="AJ18">
+        <v>19850129.52416667</v>
+      </c>
+      <c r="AK18">
+        <v>14530813.76833333</v>
+      </c>
+      <c r="AL18">
         <v>10898110.32625</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>7265406.884166666</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>3632703.442083333</v>
       </c>
     </row>
@@ -6164,15 +6502,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -6288,10 +6626,13 @@
       <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -6366,9 +6707,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -6443,9 +6784,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -6520,9 +6861,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -6597,9 +6938,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -6674,9 +7015,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -6751,9 +7092,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -6828,9 +7169,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -6905,9 +7246,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -6982,9 +7323,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -7059,9 +7400,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -7136,9 +7477,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -7213,9 +7554,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14">
         <v>2257689781.774583</v>
@@ -7290,9 +7631,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:40">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O15">
         <v>2257689781.774583</v>
@@ -7367,9 +7708,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P16">
         <v>2257689781.774583</v>
@@ -7444,122 +7785,202 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:40">
       <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="Q17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="R17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="S17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="T17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AM17">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AN17">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C18">
         <v>5666323581.648334</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>8499485372.4725</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>11332647163.29667</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>14165808954.12083</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>16998970744.945</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>19832132535.76917</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>22665294326.59333</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>25498456117.4175</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>28331617908.24166</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>31164779699.06583</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>33997941489.89</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>36255631271.66458</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>38513321053.43916</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>40771010835.21375</v>
       </c>
-      <c r="Q17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="R17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="S17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="T17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="U17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="V17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="W17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="X17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="Y17">
-        <v>40771010835.21375</v>
-      </c>
-      <c r="Z17">
-        <v>37937849044.38958</v>
-      </c>
-      <c r="AA17">
-        <v>35104687253.56541</v>
-      </c>
-      <c r="AB17">
-        <v>32271525462.74125</v>
-      </c>
-      <c r="AC17">
-        <v>29438363671.91708</v>
-      </c>
-      <c r="AD17">
-        <v>26605201881.09291</v>
-      </c>
-      <c r="AE17">
-        <v>23772040090.26875</v>
-      </c>
-      <c r="AF17">
-        <v>20938878299.44458</v>
-      </c>
-      <c r="AG17">
-        <v>18105716508.62042</v>
-      </c>
-      <c r="AH17">
-        <v>15272554717.79625</v>
-      </c>
-      <c r="AI17">
-        <v>12439392926.97208</v>
-      </c>
-      <c r="AJ17">
-        <v>9606231136.147917</v>
-      </c>
-      <c r="AK17">
+      <c r="Q18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="R18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="S18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="T18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="U18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="V18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="W18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="X18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="Y18">
+        <v>43028700616.98833</v>
+      </c>
+      <c r="Z18">
+        <v>40195538826.16416</v>
+      </c>
+      <c r="AA18">
+        <v>37362377035.34</v>
+      </c>
+      <c r="AB18">
+        <v>34529215244.51583</v>
+      </c>
+      <c r="AC18">
+        <v>31696053453.69166</v>
+      </c>
+      <c r="AD18">
+        <v>28862891662.8675</v>
+      </c>
+      <c r="AE18">
+        <v>26029729872.04333</v>
+      </c>
+      <c r="AF18">
+        <v>23196568081.21917</v>
+      </c>
+      <c r="AG18">
+        <v>20363406290.395</v>
+      </c>
+      <c r="AH18">
+        <v>17530244499.57084</v>
+      </c>
+      <c r="AI18">
+        <v>14697082708.74667</v>
+      </c>
+      <c r="AJ18">
+        <v>11863920917.9225</v>
+      </c>
+      <c r="AK18">
+        <v>9030759127.098333</v>
+      </c>
+      <c r="AL18">
         <v>6773069345.32375</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>4515379563.549167</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>2257689781.774583</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2 result in 1022
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="63">
   <si>
     <t>20210618</t>
   </si>
@@ -140,6 +140,12 @@
     <t>20220318</t>
   </si>
   <si>
+    <t>20220325</t>
+  </si>
+  <si>
+    <t>20220401</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -192,6 +198,12 @@
   </si>
   <si>
     <t>20211001-20211008</t>
+  </si>
+  <si>
+    <t>20211008-20211015</t>
+  </si>
+  <si>
+    <t>20211015-20211022</t>
   </si>
   <si>
     <t>SUM</t>
@@ -552,15 +564,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -682,10 +694,16 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41">
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -760,9 +778,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -837,9 +855,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -914,9 +932,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -991,9 +1009,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1068,9 +1086,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1145,9 +1163,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1222,9 +1240,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1299,9 +1317,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1376,9 +1394,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1453,9 +1471,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1530,9 +1548,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1607,9 +1625,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N14">
         <v>422993.89125</v>
@@ -1684,9 +1702,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O15">
         <v>422993.89125</v>
@@ -1761,9 +1779,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P16">
         <v>422993.89125</v>
@@ -1838,9 +1856,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>422993.89125</v>
@@ -1915,9 +1933,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R18">
         <v>422993.89125</v>
@@ -1992,128 +2010,288 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19">
-        <v>939796.0891666667</v>
-      </c>
-      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="S19">
+        <v>422993.89125</v>
+      </c>
+      <c r="T19">
+        <v>422993.89125</v>
+      </c>
+      <c r="U19">
+        <v>422993.89125</v>
+      </c>
+      <c r="V19">
+        <v>422993.89125</v>
+      </c>
+      <c r="W19">
+        <v>422993.89125</v>
+      </c>
+      <c r="X19">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y19">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AM19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AN19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AO19">
+        <v>422993.89125</v>
+      </c>
+      <c r="AP19">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>422993.89125</v>
+      </c>
+      <c r="U20">
+        <v>422993.89125</v>
+      </c>
+      <c r="V20">
+        <v>422993.89125</v>
+      </c>
+      <c r="W20">
+        <v>422993.89125</v>
+      </c>
+      <c r="X20">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y20">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AM20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AN20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AO20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AP20">
+        <v>422993.89125</v>
+      </c>
+      <c r="AQ20">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>939796.0891666667</v>
+      </c>
+      <c r="C21">
         <v>1879592.178333333</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>2819388.2675</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>3759184.356666667</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>4801479.284583334</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>5843774.2125</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>6886069.140416667</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>7928364.068333333</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>8765438.304583333</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>9602512.540833334</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>10439586.77708333</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>11276661.01333333</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>11699654.90458333</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>12122648.79583333</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>12545642.68708333</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>12968636.57833333</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>13391630.46958333</v>
       </c>
-      <c r="S19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="T19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="U19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="V19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="W19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="X19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="Y19">
-        <v>13391630.46958333</v>
-      </c>
-      <c r="Z19">
-        <v>12451834.38041666</v>
-      </c>
-      <c r="AA19">
-        <v>11512038.29125</v>
-      </c>
-      <c r="AB19">
-        <v>10572242.20208333</v>
-      </c>
-      <c r="AC19">
-        <v>9632446.112916665</v>
-      </c>
-      <c r="AD19">
-        <v>8590151.185000001</v>
-      </c>
-      <c r="AE19">
-        <v>7547856.257083335</v>
-      </c>
-      <c r="AF19">
-        <v>6505561.329166668</v>
-      </c>
-      <c r="AG19">
-        <v>5463266.401250001</v>
-      </c>
-      <c r="AH19">
-        <v>4626192.165</v>
-      </c>
-      <c r="AI19">
-        <v>3789117.92875</v>
-      </c>
-      <c r="AJ19">
-        <v>2952043.6925</v>
-      </c>
-      <c r="AK19">
+      <c r="S21">
+        <v>13814624.36083333</v>
+      </c>
+      <c r="T21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="U21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="V21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="W21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="X21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="Y21">
+        <v>14237618.25208333</v>
+      </c>
+      <c r="Z21">
+        <v>13297822.16291666</v>
+      </c>
+      <c r="AA21">
+        <v>12358026.07374999</v>
+      </c>
+      <c r="AB21">
+        <v>11418229.98458333</v>
+      </c>
+      <c r="AC21">
+        <v>10478433.89541666</v>
+      </c>
+      <c r="AD21">
+        <v>9436138.967499999</v>
+      </c>
+      <c r="AE21">
+        <v>8393844.039583335</v>
+      </c>
+      <c r="AF21">
+        <v>7351549.111666669</v>
+      </c>
+      <c r="AG21">
+        <v>6309254.183750002</v>
+      </c>
+      <c r="AH21">
+        <v>5472179.947500001</v>
+      </c>
+      <c r="AI21">
+        <v>4635105.711250001</v>
+      </c>
+      <c r="AJ21">
+        <v>3798031.475</v>
+      </c>
+      <c r="AK21">
+        <v>2960957.23875</v>
+      </c>
+      <c r="AL21">
+        <v>2537963.3475</v>
+      </c>
+      <c r="AM21">
         <v>2114969.45625</v>
       </c>
-      <c r="AL19">
+      <c r="AN21">
         <v>1691975.565</v>
       </c>
-      <c r="AM19">
+      <c r="AO21">
         <v>1268981.67375</v>
       </c>
-      <c r="AN19">
+      <c r="AP21">
         <v>845987.7825000001</v>
       </c>
-      <c r="AO19">
+      <c r="AQ21">
         <v>422993.89125</v>
       </c>
     </row>
@@ -2124,15 +2302,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2254,10 +2432,16 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41">
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -2332,9 +2516,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -2409,9 +2593,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2486,9 +2670,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2563,9 +2747,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2640,9 +2824,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2717,9 +2901,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -2794,9 +2978,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -2871,9 +3055,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -2948,9 +3132,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -3025,9 +3209,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -3102,9 +3286,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -3179,9 +3363,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N14">
         <v>701978.0920833334</v>
@@ -3256,9 +3440,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O15">
         <v>701978.0920833334</v>
@@ -3333,9 +3517,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P16">
         <v>701978.0920833334</v>
@@ -3410,9 +3594,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>701978.0920833334</v>
@@ -3487,9 +3671,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R18">
         <v>701978.0920833334</v>
@@ -3564,128 +3748,288 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="S19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="T19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AM19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AN19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AO19">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AP19">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="U20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="V20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AM20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AN20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AO20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AP20">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AQ20">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
         <v>942083.3333333334</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>1829625</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>2717166.666666667</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>3604708.333333333</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>4477375</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>5350041.666666667</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>6222708.333333334</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>7095375.000000001</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>8022583.333333334</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>9004333.333333334</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>9986083.333333334</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>10967833.33333333</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>11669811.42541667</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>12371789.5175</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>13073767.60958333</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>13775745.70166667</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>14477723.79375</v>
       </c>
-      <c r="S19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="T19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="U19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="V19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="W19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="X19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="Y19">
-        <v>14477723.79375</v>
-      </c>
-      <c r="Z19">
-        <v>13535640.46041667</v>
-      </c>
-      <c r="AA19">
-        <v>12648098.79375</v>
-      </c>
-      <c r="AB19">
-        <v>11760557.12708333</v>
-      </c>
-      <c r="AC19">
-        <v>10873015.46041667</v>
-      </c>
-      <c r="AD19">
-        <v>10000348.79375</v>
-      </c>
-      <c r="AE19">
-        <v>9127682.127083331</v>
-      </c>
-      <c r="AF19">
-        <v>8255015.460416665</v>
-      </c>
-      <c r="AG19">
-        <v>7382348.793749999</v>
-      </c>
-      <c r="AH19">
-        <v>6455140.460416666</v>
-      </c>
-      <c r="AI19">
-        <v>5473390.460416667</v>
-      </c>
-      <c r="AJ19">
-        <v>4491640.460416667</v>
-      </c>
-      <c r="AK19">
+      <c r="S21">
+        <v>15179701.88583333</v>
+      </c>
+      <c r="T21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="U21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="V21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="W21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="X21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="Y21">
+        <v>15881679.97791667</v>
+      </c>
+      <c r="Z21">
+        <v>14939596.64458333</v>
+      </c>
+      <c r="AA21">
+        <v>14052054.97791666</v>
+      </c>
+      <c r="AB21">
+        <v>13164513.31125</v>
+      </c>
+      <c r="AC21">
+        <v>12276971.64458333</v>
+      </c>
+      <c r="AD21">
+        <v>11404304.97791667</v>
+      </c>
+      <c r="AE21">
+        <v>10531638.31125</v>
+      </c>
+      <c r="AF21">
+        <v>9658971.644583331</v>
+      </c>
+      <c r="AG21">
+        <v>8786304.977916665</v>
+      </c>
+      <c r="AH21">
+        <v>7859096.644583332</v>
+      </c>
+      <c r="AI21">
+        <v>6877346.644583333</v>
+      </c>
+      <c r="AJ21">
+        <v>5895596.644583333</v>
+      </c>
+      <c r="AK21">
+        <v>4913846.644583333</v>
+      </c>
+      <c r="AL21">
+        <v>4211868.5525</v>
+      </c>
+      <c r="AM21">
         <v>3509890.460416667</v>
       </c>
-      <c r="AL19">
+      <c r="AN21">
         <v>2807912.368333334</v>
       </c>
-      <c r="AM19">
+      <c r="AO21">
         <v>2105934.27625</v>
       </c>
-      <c r="AN19">
+      <c r="AP21">
         <v>1403956.184166667</v>
       </c>
-      <c r="AO19">
+      <c r="AQ21">
         <v>701978.0920833334</v>
       </c>
     </row>
@@ -3696,15 +4040,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3826,10 +4170,16 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41">
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -3904,9 +4254,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -3981,9 +4331,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -4058,9 +4408,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -4135,9 +4485,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -4212,9 +4562,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -4289,9 +4639,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -4366,9 +4716,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -4443,9 +4793,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -4520,9 +4870,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -4597,9 +4947,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -4674,9 +5024,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -4751,9 +5101,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N14">
         <v>1513058.30375</v>
@@ -4828,9 +5178,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O15">
         <v>1513058.30375</v>
@@ -4905,9 +5255,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P16">
         <v>1513058.30375</v>
@@ -4982,9 +5332,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>1513058.30375</v>
@@ -5059,9 +5409,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R18">
         <v>1513058.30375</v>
@@ -5136,128 +5486,288 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="S19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="T19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AM19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AN19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AO19">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AP19">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="U20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="V20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AM20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AN20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AO20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AP20">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AQ20">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C21">
         <v>4045953.864166667</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>6068930.796250001</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>8091907.728333334</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>10114884.66041667</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>12137861.5925</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>14160838.52458333</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>16183815.45666667</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>18206792.38875</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>20229769.32083334</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>22252746.25291667</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>24275723.18500001</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>25788781.48875001</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>27301839.79250001</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>28814898.09625001</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>30327956.40000001</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>31841014.70375001</v>
       </c>
-      <c r="S19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="T19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="U19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="V19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="W19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="X19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="Y19">
-        <v>31841014.70375001</v>
-      </c>
-      <c r="Z19">
-        <v>29818037.77166668</v>
-      </c>
-      <c r="AA19">
-        <v>27795060.83958334</v>
-      </c>
-      <c r="AB19">
-        <v>25772083.90750001</v>
-      </c>
-      <c r="AC19">
-        <v>23749106.97541667</v>
-      </c>
-      <c r="AD19">
-        <v>21726130.04333334</v>
-      </c>
-      <c r="AE19">
-        <v>19703153.11125001</v>
-      </c>
-      <c r="AF19">
-        <v>17680176.17916667</v>
-      </c>
-      <c r="AG19">
-        <v>15657199.24708334</v>
-      </c>
-      <c r="AH19">
-        <v>13634222.315</v>
-      </c>
-      <c r="AI19">
-        <v>11611245.38291667</v>
-      </c>
-      <c r="AJ19">
-        <v>9588268.450833334</v>
-      </c>
-      <c r="AK19">
+      <c r="S21">
+        <v>33354073.00750001</v>
+      </c>
+      <c r="T21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="U21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="V21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="W21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="X21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="Y21">
+        <v>34867131.31125001</v>
+      </c>
+      <c r="Z21">
+        <v>32844154.37916668</v>
+      </c>
+      <c r="AA21">
+        <v>30821177.44708334</v>
+      </c>
+      <c r="AB21">
+        <v>28798200.51500001</v>
+      </c>
+      <c r="AC21">
+        <v>26775223.58291667</v>
+      </c>
+      <c r="AD21">
+        <v>24752246.65083334</v>
+      </c>
+      <c r="AE21">
+        <v>22729269.71875001</v>
+      </c>
+      <c r="AF21">
+        <v>20706292.78666667</v>
+      </c>
+      <c r="AG21">
+        <v>18683315.85458334</v>
+      </c>
+      <c r="AH21">
+        <v>16660338.9225</v>
+      </c>
+      <c r="AI21">
+        <v>14637361.99041667</v>
+      </c>
+      <c r="AJ21">
+        <v>12614385.05833333</v>
+      </c>
+      <c r="AK21">
+        <v>10591408.12625</v>
+      </c>
+      <c r="AL21">
+        <v>9078349.8225</v>
+      </c>
+      <c r="AM21">
         <v>7565291.51875</v>
       </c>
-      <c r="AL19">
+      <c r="AN21">
         <v>6052233.215</v>
       </c>
-      <c r="AM19">
+      <c r="AO21">
         <v>4539174.91125</v>
       </c>
-      <c r="AN19">
+      <c r="AP21">
         <v>3026116.6075</v>
       </c>
-      <c r="AO19">
+      <c r="AQ21">
         <v>1513058.30375</v>
       </c>
     </row>
@@ -5268,15 +5778,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5398,10 +5908,16 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41">
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -5476,9 +5992,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -5553,9 +6069,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -5630,9 +6146,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -5707,9 +6223,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -5784,9 +6300,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -5861,9 +6377,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -5938,9 +6454,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -6015,9 +6531,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -6092,9 +6608,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -6169,9 +6685,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -6246,9 +6762,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -6323,9 +6839,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N14">
         <v>3632703.442083333</v>
@@ -6400,9 +6916,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O15">
         <v>3632703.442083333</v>
@@ -6477,9 +6993,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P16">
         <v>3632703.442083333</v>
@@ -6554,9 +7070,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>3632703.442083333</v>
@@ -6631,9 +7147,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R18">
         <v>3632703.442083333</v>
@@ -6708,128 +7224,288 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="S19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="T19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AM19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AN19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AO19">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AP19">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="U20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="V20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AM20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AN20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AO20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AP20">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AQ20">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C21">
         <v>10638631.51166667</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>15957947.2675</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>21277263.02333333</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>26596578.77916667</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>31915894.535</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>37235210.29083334</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>42554526.04666667</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>47873841.80250001</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>53193157.55833334</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>58512473.31416668</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>63831789.07000002</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>67464492.51208335</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>71097195.95416668</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>74729899.39625001</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>78362602.83833334</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>81995306.28041667</v>
       </c>
-      <c r="S19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="T19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="U19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="V19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="W19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="X19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="Y19">
-        <v>81995306.28041667</v>
-      </c>
-      <c r="Z19">
-        <v>76675990.52458334</v>
-      </c>
-      <c r="AA19">
-        <v>71356674.76875001</v>
-      </c>
-      <c r="AB19">
-        <v>66037359.01291669</v>
-      </c>
-      <c r="AC19">
-        <v>60718043.25708336</v>
-      </c>
-      <c r="AD19">
-        <v>55398727.50125002</v>
-      </c>
-      <c r="AE19">
-        <v>50079411.74541669</v>
-      </c>
-      <c r="AF19">
-        <v>44760095.98958334</v>
-      </c>
-      <c r="AG19">
-        <v>39440780.23375</v>
-      </c>
-      <c r="AH19">
-        <v>34121464.47791667</v>
-      </c>
-      <c r="AI19">
-        <v>28802148.72208333</v>
-      </c>
-      <c r="AJ19">
-        <v>23482832.96625</v>
-      </c>
-      <c r="AK19">
+      <c r="S21">
+        <v>85628009.7225</v>
+      </c>
+      <c r="T21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="U21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="V21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="W21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="X21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="Y21">
+        <v>89260713.16458333</v>
+      </c>
+      <c r="Z21">
+        <v>83941397.40875</v>
+      </c>
+      <c r="AA21">
+        <v>78622081.65291667</v>
+      </c>
+      <c r="AB21">
+        <v>73302765.89708336</v>
+      </c>
+      <c r="AC21">
+        <v>67983450.14125003</v>
+      </c>
+      <c r="AD21">
+        <v>62664134.38541669</v>
+      </c>
+      <c r="AE21">
+        <v>57344818.62958336</v>
+      </c>
+      <c r="AF21">
+        <v>52025502.87375002</v>
+      </c>
+      <c r="AG21">
+        <v>46706187.11791667</v>
+      </c>
+      <c r="AH21">
+        <v>41386871.36208334</v>
+      </c>
+      <c r="AI21">
+        <v>36067555.60625</v>
+      </c>
+      <c r="AJ21">
+        <v>30748239.85041666</v>
+      </c>
+      <c r="AK21">
+        <v>25428924.09458333</v>
+      </c>
+      <c r="AL21">
+        <v>21796220.6525</v>
+      </c>
+      <c r="AM21">
         <v>18163517.21041667</v>
       </c>
-      <c r="AL19">
+      <c r="AN21">
         <v>14530813.76833333</v>
       </c>
-      <c r="AM19">
+      <c r="AO21">
         <v>10898110.32625</v>
       </c>
-      <c r="AN19">
+      <c r="AP21">
         <v>7265406.884166666</v>
       </c>
-      <c r="AO19">
+      <c r="AQ21">
         <v>3632703.442083333</v>
       </c>
     </row>
@@ -6840,15 +7516,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -6970,10 +7646,16 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41">
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -7048,9 +7730,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -7125,9 +7807,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -7202,9 +7884,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -7279,9 +7961,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -7356,9 +8038,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -7433,9 +8115,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -7510,9 +8192,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -7587,9 +8269,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -7664,9 +8346,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -7741,9 +8423,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -7818,9 +8500,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -7895,9 +8577,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N14">
         <v>2257689781.774583</v>
@@ -7972,9 +8654,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O15">
         <v>2257689781.774583</v>
@@ -8049,9 +8731,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P16">
         <v>2257689781.774583</v>
@@ -8126,9 +8808,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>2257689781.774583</v>
@@ -8203,9 +8885,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R18">
         <v>2257689781.774583</v>
@@ -8280,128 +8962,288 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="S19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="T19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AM19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AN19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AO19">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AP19">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="U20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="V20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AM20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AN20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AO20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AP20">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AQ20">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C21">
         <v>5666323581.648334</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>8499485372.4725</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>11332647163.29667</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>14165808954.12083</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>16998970744.945</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>19832132535.76917</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>22665294326.59333</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>25498456117.4175</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>28331617908.24166</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>31164779699.06583</v>
       </c>
-      <c r="M19">
+      <c r="M21">
         <v>33997941489.89</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>36255631271.66458</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>38513321053.43916</v>
       </c>
-      <c r="P19">
+      <c r="P21">
         <v>40771010835.21375</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <v>43028700616.98833</v>
       </c>
-      <c r="R19">
+      <c r="R21">
         <v>45286390398.76291</v>
       </c>
-      <c r="S19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="T19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="U19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="V19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="W19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="X19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="Y19">
-        <v>45286390398.76291</v>
-      </c>
-      <c r="Z19">
-        <v>42453228607.93874</v>
-      </c>
-      <c r="AA19">
-        <v>39620066817.11458</v>
-      </c>
-      <c r="AB19">
-        <v>36786905026.29041</v>
-      </c>
-      <c r="AC19">
-        <v>33953743235.46624</v>
-      </c>
-      <c r="AD19">
-        <v>31120581444.64208</v>
-      </c>
-      <c r="AE19">
-        <v>28287419653.81791</v>
-      </c>
-      <c r="AF19">
-        <v>25454257862.99375</v>
-      </c>
-      <c r="AG19">
-        <v>22621096072.16958</v>
-      </c>
-      <c r="AH19">
-        <v>19787934281.34542</v>
-      </c>
-      <c r="AI19">
-        <v>16954772490.52125</v>
-      </c>
-      <c r="AJ19">
-        <v>14121610699.69708</v>
-      </c>
-      <c r="AK19">
+      <c r="S21">
+        <v>47544080180.53749</v>
+      </c>
+      <c r="T21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="U21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="V21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="W21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="X21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="Y21">
+        <v>49801769962.31207</v>
+      </c>
+      <c r="Z21">
+        <v>46968608171.48791</v>
+      </c>
+      <c r="AA21">
+        <v>44135446380.66374</v>
+      </c>
+      <c r="AB21">
+        <v>41302284589.83958</v>
+      </c>
+      <c r="AC21">
+        <v>38469122799.01541</v>
+      </c>
+      <c r="AD21">
+        <v>35635961008.19125</v>
+      </c>
+      <c r="AE21">
+        <v>32802799217.36708</v>
+      </c>
+      <c r="AF21">
+        <v>29969637426.54291</v>
+      </c>
+      <c r="AG21">
+        <v>27136475635.71875</v>
+      </c>
+      <c r="AH21">
+        <v>24303313844.89458</v>
+      </c>
+      <c r="AI21">
+        <v>21470152054.07042</v>
+      </c>
+      <c r="AJ21">
+        <v>18636990263.24625</v>
+      </c>
+      <c r="AK21">
+        <v>15803828472.42208</v>
+      </c>
+      <c r="AL21">
+        <v>13546138690.6475</v>
+      </c>
+      <c r="AM21">
         <v>11288448908.87292</v>
       </c>
-      <c r="AL19">
+      <c r="AN21">
         <v>9030759127.098333</v>
       </c>
-      <c r="AM19">
+      <c r="AO21">
         <v>6773069345.32375</v>
       </c>
-      <c r="AN19">
+      <c r="AP21">
         <v>4515379563.549167</v>
       </c>
-      <c r="AO19">
+      <c r="AQ21">
         <v>2257689781.774583</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1105 & 1112 v2
</commit_message>
<xml_diff>
--- a/theoretical_airdrop.xlsx
+++ b/theoretical_airdrop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="69">
   <si>
     <t>20210618</t>
   </si>
@@ -149,6 +149,12 @@
     <t>20220408</t>
   </si>
   <si>
+    <t>20220415</t>
+  </si>
+  <si>
+    <t>20220422</t>
+  </si>
+  <si>
     <t>period</t>
   </si>
   <si>
@@ -210,6 +216,12 @@
   </si>
   <si>
     <t>20211022-20211029</t>
+  </si>
+  <si>
+    <t>20211029-20211105</t>
+  </si>
+  <si>
+    <t>20211105-20211112</t>
   </si>
   <si>
     <t>SUM</t>
@@ -570,15 +582,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR22"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -709,10 +721,16 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>939796.0891666667</v>
@@ -787,9 +805,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>939796.0891666667</v>
@@ -864,9 +882,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>939796.0891666667</v>
@@ -941,9 +959,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>939796.0891666667</v>
@@ -1018,9 +1036,9 @@
         <v>939796.0891666667</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:46">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>1042294.927916667</v>
@@ -1095,9 +1113,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:46">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7">
         <v>1042294.927916667</v>
@@ -1172,9 +1190,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:46">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>1042294.927916667</v>
@@ -1249,9 +1267,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:46">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>1042294.927916667</v>
@@ -1326,9 +1344,9 @@
         <v>1042294.927916667</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:46">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>837074.2362500001</v>
@@ -1403,9 +1421,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:46">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>837074.2362500001</v>
@@ -1480,9 +1498,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:46">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>837074.2362500001</v>
@@ -1557,9 +1575,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>837074.2362500001</v>
@@ -1634,9 +1652,9 @@
         <v>837074.2362500001</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:46">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>422993.89125</v>
@@ -1711,9 +1729,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:46">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>422993.89125</v>
@@ -1788,9 +1806,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:46">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16">
         <v>422993.89125</v>
@@ -1865,9 +1883,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:46">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <v>422993.89125</v>
@@ -1942,9 +1960,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:46">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R18">
         <v>422993.89125</v>
@@ -2019,9 +2037,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:46">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S19">
         <v>422993.89125</v>
@@ -2096,9 +2114,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:46">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20">
         <v>422993.89125</v>
@@ -2173,9 +2191,9 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:46">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U21">
         <v>422993.89125</v>
@@ -2250,138 +2268,298 @@
         <v>422993.89125</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:46">
       <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>422993.89125</v>
+      </c>
+      <c r="W22">
+        <v>422993.89125</v>
+      </c>
+      <c r="X22">
+        <v>422993.89125</v>
+      </c>
+      <c r="Y22">
+        <v>422993.89125</v>
+      </c>
+      <c r="Z22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AA22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AB22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AC22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AD22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AE22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AF22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AG22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AH22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AI22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AJ22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AK22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AL22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AM22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AN22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AO22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AP22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AQ22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AR22">
+        <v>422993.89125</v>
+      </c>
+      <c r="AS22">
+        <v>422993.89125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
         <v>939796.0891666667</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>1879592.178333333</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>2819388.2675</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>3759184.356666667</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>4801479.284583334</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>5843774.2125</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>6886069.140416667</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>7928364.068333333</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>8765438.304583333</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>9602512.540833334</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>10439586.77708333</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>11276661.01333333</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>11699654.90458333</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>12122648.79583333</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>12545642.68708333</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>12968636.57833333</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>13391630.46958333</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>13814624.36083333</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>14237618.25208333</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>14660612.14333333</v>
       </c>
-      <c r="V22">
-        <v>14660612.14333333</v>
-      </c>
-      <c r="W22">
-        <v>14660612.14333333</v>
-      </c>
-      <c r="X22">
-        <v>14660612.14333333</v>
-      </c>
-      <c r="Y22">
-        <v>14660612.14333333</v>
-      </c>
-      <c r="Z22">
-        <v>13720816.05416666</v>
-      </c>
-      <c r="AA22">
-        <v>12781019.96499999</v>
-      </c>
-      <c r="AB22">
-        <v>11841223.87583333</v>
-      </c>
-      <c r="AC22">
-        <v>10901427.78666666</v>
-      </c>
-      <c r="AD22">
-        <v>9859132.858749999</v>
-      </c>
-      <c r="AE22">
-        <v>8816837.930833334</v>
-      </c>
-      <c r="AF22">
-        <v>7774543.002916669</v>
-      </c>
-      <c r="AG22">
-        <v>6732248.075000002</v>
-      </c>
-      <c r="AH22">
-        <v>5895173.838750001</v>
-      </c>
-      <c r="AI22">
-        <v>5058099.602500001</v>
-      </c>
-      <c r="AJ22">
-        <v>4221025.36625</v>
-      </c>
-      <c r="AK22">
+      <c r="V24">
+        <v>15083606.03458333</v>
+      </c>
+      <c r="W24">
+        <v>15083606.03458333</v>
+      </c>
+      <c r="X24">
+        <v>15083606.03458333</v>
+      </c>
+      <c r="Y24">
+        <v>15083606.03458333</v>
+      </c>
+      <c r="Z24">
+        <v>14143809.94541666</v>
+      </c>
+      <c r="AA24">
+        <v>13204013.85624999</v>
+      </c>
+      <c r="AB24">
+        <v>12264217.76708333</v>
+      </c>
+      <c r="AC24">
+        <v>11324421.67791666</v>
+      </c>
+      <c r="AD24">
+        <v>10282126.75</v>
+      </c>
+      <c r="AE24">
+        <v>9239831.822083334</v>
+      </c>
+      <c r="AF24">
+        <v>8197536.89416667</v>
+      </c>
+      <c r="AG24">
+        <v>7155241.966250002</v>
+      </c>
+      <c r="AH24">
+        <v>6318167.730000001</v>
+      </c>
+      <c r="AI24">
+        <v>5481093.493750001</v>
+      </c>
+      <c r="AJ24">
+        <v>4644019.2575</v>
+      </c>
+      <c r="AK24">
+        <v>3806945.02125</v>
+      </c>
+      <c r="AL24">
         <v>3383951.13</v>
       </c>
-      <c r="AL22">
+      <c r="AM24">
         <v>2960957.23875</v>
       </c>
-      <c r="AM22">
+      <c r="AN24">
         <v>2537963.3475</v>
       </c>
-      <c r="AN22">
+      <c r="AO24">
         <v>2114969.45625</v>
       </c>
-      <c r="AO22">
+      <c r="AP24">
         <v>1691975.565</v>
       </c>
-      <c r="AP22">
+      <c r="AQ24">
         <v>1268981.67375</v>
       </c>
-      <c r="AQ22">
+      <c r="AR24">
         <v>845987.7825000001</v>
       </c>
-      <c r="AR22">
-        <v>422993.89125</v>
+      <c r="AS24">
+        <v>422993.89125</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2391,15 +2569,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR22"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2530,10 +2708,16 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>942083.3333333334</v>
@@ -2608,9 +2792,9 @@
         <v>942083.3333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>887541.6666666666</v>
@@ -2685,9 +2869,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>887541.6666666666</v>
@@ -2762,9 +2946,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>887541.6666666666</v>
@@ -2839,9 +3023,9 @@
         <v>887541.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:46">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>872666.6666666666</v>
@@ -2916,9 +3100,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:46">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7">
         <v>872666.6666666666</v>
@@ -2993,9 +3177,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:46">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>872666.6666666666</v>
@@ -3070,9 +3254,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:46">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>872666.6666666666</v>
@@ -3147,9 +3331,9 @@
         <v>872666.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:46">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>927208.3333333334</v>
@@ -3224,9 +3408,9 @@
         <v>927208.3333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:46">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>981750</v>
@@ -3301,9 +3485,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:46">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>981750</v>
@@ -3378,9 +3562,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>981750</v>
@@ -3455,9 +3639,9 @@
         <v>981750</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:46">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>701978.0920833334</v>
@@ -3532,9 +3716,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:46">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>701978.0920833334</v>
@@ -3609,9 +3793,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:46">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16">
         <v>701978.0920833334</v>
@@ -3686,9 +3870,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:46">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <v>701978.0920833334</v>
@@ -3763,9 +3947,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:46">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R18">
         <v>701978.0920833334</v>
@@ -3840,9 +4024,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:46">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S19">
         <v>701978.0920833334</v>
@@ -3917,9 +4101,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:46">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20">
         <v>701978.0920833334</v>
@@ -3994,9 +4178,9 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:46">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U21">
         <v>701978.0920833334</v>
@@ -4071,138 +4255,298 @@
         <v>701978.0920833334</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:46">
       <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="W22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="X22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Y22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="Z22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AA22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AB22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AC22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AD22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AE22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AF22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AG22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AH22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AI22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AJ22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AK22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AL22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AM22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AN22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AO22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AP22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AQ22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AR22">
+        <v>701978.0920833334</v>
+      </c>
+      <c r="AS22">
+        <v>701978.0920833334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="X23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="Y23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="Z23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AA23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AB23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AC23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AD23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AE23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AF23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AG23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AH23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AI23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AJ23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AK23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AL23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AM23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AN23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AO23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AP23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AQ23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AR23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AS23">
+        <v>524710.9583333334</v>
+      </c>
+      <c r="AT23">
+        <v>524710.9583333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
         <v>942083.3333333334</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>1829625</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>2717166.666666667</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>3604708.333333333</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>4477375</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>5350041.666666667</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>6222708.333333334</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>7095375.000000001</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>8022583.333333334</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>9004333.333333334</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>9986083.333333334</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>10967833.33333333</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>11669811.42541667</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>12371789.5175</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>13073767.60958333</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>13775745.70166667</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>14477723.79375</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>15179701.88583333</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>15881679.97791667</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>16583658.07</v>
       </c>
-      <c r="V22">
-        <v>16583658.07</v>
-      </c>
-      <c r="W22">
-        <v>16583658.07</v>
-      </c>
-      <c r="X22">
-        <v>16583658.07</v>
-      </c>
-      <c r="Y22">
-        <v>16583658.07</v>
-      </c>
-      <c r="Z22">
-        <v>15641574.73666666</v>
-      </c>
-      <c r="AA22">
-        <v>14754033.07</v>
-      </c>
-      <c r="AB22">
-        <v>13866491.40333333</v>
-      </c>
-      <c r="AC22">
-        <v>12978949.73666666</v>
-      </c>
-      <c r="AD22">
-        <v>12106283.07</v>
-      </c>
-      <c r="AE22">
-        <v>11233616.40333333</v>
-      </c>
-      <c r="AF22">
-        <v>10360949.73666666</v>
-      </c>
-      <c r="AG22">
-        <v>9488283.069999998</v>
-      </c>
-      <c r="AH22">
-        <v>8561074.736666666</v>
-      </c>
-      <c r="AI22">
-        <v>7579324.736666666</v>
-      </c>
-      <c r="AJ22">
-        <v>6597574.736666666</v>
-      </c>
-      <c r="AK22">
-        <v>5615824.736666666</v>
-      </c>
-      <c r="AL22">
-        <v>4913846.644583333</v>
-      </c>
-      <c r="AM22">
-        <v>4211868.5525</v>
-      </c>
-      <c r="AN22">
-        <v>3509890.460416667</v>
-      </c>
-      <c r="AO22">
-        <v>2807912.368333334</v>
-      </c>
-      <c r="AP22">
-        <v>2105934.27625</v>
-      </c>
-      <c r="AQ22">
-        <v>1403956.184166667</v>
-      </c>
-      <c r="AR22">
-        <v>701978.0920833334</v>
+      <c r="V24">
+        <v>17285636.16208333</v>
+      </c>
+      <c r="W24">
+        <v>17810347.12041666</v>
+      </c>
+      <c r="X24">
+        <v>17810347.12041666</v>
+      </c>
+      <c r="Y24">
+        <v>17810347.12041666</v>
+      </c>
+      <c r="Z24">
+        <v>16868263.78708333</v>
+      </c>
+      <c r="AA24">
+        <v>15980722.12041666</v>
+      </c>
+      <c r="AB24">
+        <v>15093180.45375</v>
+      </c>
+      <c r="AC24">
+        <v>14205638.78708333</v>
+      </c>
+      <c r="AD24">
+        <v>13332972.12041667</v>
+      </c>
+      <c r="AE24">
+        <v>12460305.45375</v>
+      </c>
+      <c r="AF24">
+        <v>11587638.78708333</v>
+      </c>
+      <c r="AG24">
+        <v>10714972.12041667</v>
+      </c>
+      <c r="AH24">
+        <v>9787763.787083333</v>
+      </c>
+      <c r="AI24">
+        <v>8806013.787083333</v>
+      </c>
+      <c r="AJ24">
+        <v>7824263.787083332</v>
+      </c>
+      <c r="AK24">
+        <v>6842513.787083332</v>
+      </c>
+      <c r="AL24">
+        <v>6140535.694999999</v>
+      </c>
+      <c r="AM24">
+        <v>5438557.602916666</v>
+      </c>
+      <c r="AN24">
+        <v>4736579.510833333</v>
+      </c>
+      <c r="AO24">
+        <v>4034601.418750001</v>
+      </c>
+      <c r="AP24">
+        <v>3332623.326666667</v>
+      </c>
+      <c r="AQ24">
+        <v>2630645.234583334</v>
+      </c>
+      <c r="AR24">
+        <v>1928667.1425</v>
+      </c>
+      <c r="AS24">
+        <v>1226689.050416667</v>
+      </c>
+      <c r="AT24">
+        <v>524710.9583333334</v>
       </c>
     </row>
   </sheetData>
@@ -4212,15 +4556,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR22"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4351,10 +4695,16 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>2022976.932083334</v>
@@ -4429,9 +4779,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>2022976.932083334</v>
@@ -4506,9 +4856,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>2022976.932083334</v>
@@ -4583,9 +4933,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>2022976.932083334</v>
@@ -4660,9 +5010,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:46">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>2022976.932083334</v>
@@ -4737,9 +5087,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:46">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7">
         <v>2022976.932083334</v>
@@ -4814,9 +5164,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:46">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>2022976.932083334</v>
@@ -4891,9 +5241,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:46">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>2022976.932083334</v>
@@ -4968,9 +5318,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:46">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>2022976.932083334</v>
@@ -5045,9 +5395,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:46">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>2022976.932083334</v>
@@ -5122,9 +5472,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:46">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>2022976.932083334</v>
@@ -5199,9 +5549,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>2022976.932083334</v>
@@ -5276,9 +5626,9 @@
         <v>2022976.932083334</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:46">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>1513058.30375</v>
@@ -5353,9 +5703,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:46">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>1513058.30375</v>
@@ -5430,9 +5780,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:46">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16">
         <v>1513058.30375</v>
@@ -5507,9 +5857,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:46">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <v>1513058.30375</v>
@@ -5584,9 +5934,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:46">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R18">
         <v>1513058.30375</v>
@@ -5661,9 +6011,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:46">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S19">
         <v>1513058.30375</v>
@@ -5738,9 +6088,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:46">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20">
         <v>1513058.30375</v>
@@ -5815,9 +6165,9 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:46">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U21">
         <v>1513058.30375</v>
@@ -5892,138 +6242,298 @@
         <v>1513058.30375</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:46">
       <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
-        <v>2022976.932083334</v>
-      </c>
-      <c r="C22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="W22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="X22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Y22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="Z22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AA22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AB22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AC22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AD22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AE22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AF22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AG22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AH22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AI22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AJ22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AK22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AL22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AM22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AN22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AO22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AP22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AQ22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AR22">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AS22">
+        <v>1513058.30375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>2022976.932083334</v>
+      </c>
+      <c r="C24">
         <v>4045953.864166667</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>6068930.796250001</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>8091907.728333334</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>10114884.66041667</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>12137861.5925</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>14160838.52458333</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>16183815.45666667</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>18206792.38875</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>20229769.32083334</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>22252746.25291667</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>24275723.18500001</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>25788781.48875001</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>27301839.79250001</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>28814898.09625001</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>30327956.40000001</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>31841014.70375001</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>33354073.00750001</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>34867131.31125001</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>36380189.61500001</v>
       </c>
-      <c r="V22">
-        <v>36380189.61500001</v>
-      </c>
-      <c r="W22">
-        <v>36380189.61500001</v>
-      </c>
-      <c r="X22">
-        <v>36380189.61500001</v>
-      </c>
-      <c r="Y22">
-        <v>36380189.61500001</v>
-      </c>
-      <c r="Z22">
-        <v>34357212.68291668</v>
-      </c>
-      <c r="AA22">
-        <v>32334235.75083334</v>
-      </c>
-      <c r="AB22">
-        <v>30311258.81875001</v>
-      </c>
-      <c r="AC22">
-        <v>28288281.88666667</v>
-      </c>
-      <c r="AD22">
-        <v>26265304.95458334</v>
-      </c>
-      <c r="AE22">
-        <v>24242328.02250001</v>
-      </c>
-      <c r="AF22">
-        <v>22219351.09041667</v>
-      </c>
-      <c r="AG22">
-        <v>20196374.15833334</v>
-      </c>
-      <c r="AH22">
-        <v>18173397.22625</v>
-      </c>
-      <c r="AI22">
-        <v>16150420.29416667</v>
-      </c>
-      <c r="AJ22">
-        <v>14127443.36208333</v>
-      </c>
-      <c r="AK22">
+      <c r="V24">
+        <v>37893247.91875001</v>
+      </c>
+      <c r="W24">
+        <v>37893247.91875001</v>
+      </c>
+      <c r="X24">
+        <v>37893247.91875001</v>
+      </c>
+      <c r="Y24">
+        <v>37893247.91875001</v>
+      </c>
+      <c r="Z24">
+        <v>35870270.98666668</v>
+      </c>
+      <c r="AA24">
+        <v>33847294.05458334</v>
+      </c>
+      <c r="AB24">
+        <v>31824317.12250001</v>
+      </c>
+      <c r="AC24">
+        <v>29801340.19041668</v>
+      </c>
+      <c r="AD24">
+        <v>27778363.25833334</v>
+      </c>
+      <c r="AE24">
+        <v>25755386.32625001</v>
+      </c>
+      <c r="AF24">
+        <v>23732409.39416667</v>
+      </c>
+      <c r="AG24">
+        <v>21709432.46208334</v>
+      </c>
+      <c r="AH24">
+        <v>19686455.53</v>
+      </c>
+      <c r="AI24">
+        <v>17663478.59791667</v>
+      </c>
+      <c r="AJ24">
+        <v>15640501.66583334</v>
+      </c>
+      <c r="AK24">
+        <v>13617524.73375</v>
+      </c>
+      <c r="AL24">
         <v>12104466.43</v>
       </c>
-      <c r="AL22">
+      <c r="AM24">
         <v>10591408.12625</v>
       </c>
-      <c r="AM22">
+      <c r="AN24">
         <v>9078349.8225</v>
       </c>
-      <c r="AN22">
+      <c r="AO24">
         <v>7565291.51875</v>
       </c>
-      <c r="AO22">
+      <c r="AP24">
         <v>6052233.215</v>
       </c>
-      <c r="AP22">
+      <c r="AQ24">
         <v>4539174.91125</v>
       </c>
-      <c r="AQ22">
+      <c r="AR24">
         <v>3026116.6075</v>
       </c>
-      <c r="AR22">
-        <v>1513058.30375</v>
+      <c r="AS24">
+        <v>1513058.30375</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6033,15 +6543,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR22"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -6172,10 +6682,16 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>5319315.755833333</v>
@@ -6250,9 +6766,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>5319315.755833333</v>
@@ -6327,9 +6843,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>5319315.755833333</v>
@@ -6404,9 +6920,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>5319315.755833333</v>
@@ -6481,9 +6997,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:46">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>5319315.755833333</v>
@@ -6558,9 +7074,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:46">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7">
         <v>5319315.755833333</v>
@@ -6635,9 +7151,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:46">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>5319315.755833333</v>
@@ -6712,9 +7228,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:46">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>5319315.755833333</v>
@@ -6789,9 +7305,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:46">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>5319315.755833333</v>
@@ -6866,9 +7382,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:46">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>5319315.755833333</v>
@@ -6943,9 +7459,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:46">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>5319315.755833333</v>
@@ -7020,9 +7536,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>5319315.755833333</v>
@@ -7097,9 +7613,9 @@
         <v>5319315.755833333</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:46">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>3632703.442083333</v>
@@ -7174,9 +7690,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:46">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>3632703.442083333</v>
@@ -7251,9 +7767,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:46">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16">
         <v>3632703.442083333</v>
@@ -7328,9 +7844,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:46">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <v>3632703.442083333</v>
@@ -7405,9 +7921,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:46">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R18">
         <v>3632703.442083333</v>
@@ -7482,9 +7998,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:46">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S19">
         <v>3632703.442083333</v>
@@ -7559,9 +8075,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:46">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20">
         <v>3632703.442083333</v>
@@ -7636,9 +8152,9 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:46">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U21">
         <v>3632703.442083333</v>
@@ -7713,138 +8229,298 @@
         <v>3632703.442083333</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:46">
       <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
-        <v>5319315.755833333</v>
-      </c>
-      <c r="C22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="W22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="X22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Y22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="Z22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AA22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AB22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AC22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AD22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AE22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AF22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AG22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AH22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AI22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AJ22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AK22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AL22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AM22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AN22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AO22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AP22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AQ22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AR22">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AS22">
+        <v>3632703.442083333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>5319315.755833333</v>
+      </c>
+      <c r="C24">
         <v>10638631.51166667</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>15957947.2675</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>21277263.02333333</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>26596578.77916667</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>31915894.535</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>37235210.29083334</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>42554526.04666667</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>47873841.80250001</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>53193157.55833334</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>58512473.31416668</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>63831789.07000002</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>67464492.51208335</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>71097195.95416668</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>74729899.39625001</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>78362602.83833334</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>81995306.28041667</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>85628009.7225</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>89260713.16458333</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>92893416.60666665</v>
       </c>
-      <c r="V22">
-        <v>92893416.60666665</v>
-      </c>
-      <c r="W22">
-        <v>92893416.60666665</v>
-      </c>
-      <c r="X22">
-        <v>92893416.60666665</v>
-      </c>
-      <c r="Y22">
-        <v>92893416.60666665</v>
-      </c>
-      <c r="Z22">
-        <v>87574100.85083333</v>
-      </c>
-      <c r="AA22">
-        <v>82254785.095</v>
-      </c>
-      <c r="AB22">
-        <v>76935469.33916669</v>
-      </c>
-      <c r="AC22">
-        <v>71616153.58333336</v>
-      </c>
-      <c r="AD22">
-        <v>66296837.82750003</v>
-      </c>
-      <c r="AE22">
-        <v>60977522.0716667</v>
-      </c>
-      <c r="AF22">
-        <v>55658206.31583335</v>
-      </c>
-      <c r="AG22">
-        <v>50338890.56000001</v>
-      </c>
-      <c r="AH22">
-        <v>45019574.80416667</v>
-      </c>
-      <c r="AI22">
-        <v>39700259.04833333</v>
-      </c>
-      <c r="AJ22">
-        <v>34380943.2925</v>
-      </c>
-      <c r="AK22">
+      <c r="V24">
+        <v>96526120.04874998</v>
+      </c>
+      <c r="W24">
+        <v>96526120.04874998</v>
+      </c>
+      <c r="X24">
+        <v>96526120.04874998</v>
+      </c>
+      <c r="Y24">
+        <v>96526120.04874998</v>
+      </c>
+      <c r="Z24">
+        <v>91206804.29291666</v>
+      </c>
+      <c r="AA24">
+        <v>85887488.53708333</v>
+      </c>
+      <c r="AB24">
+        <v>80568172.78125001</v>
+      </c>
+      <c r="AC24">
+        <v>75248857.02541669</v>
+      </c>
+      <c r="AD24">
+        <v>69929541.26958336</v>
+      </c>
+      <c r="AE24">
+        <v>64610225.51375003</v>
+      </c>
+      <c r="AF24">
+        <v>59290909.75791669</v>
+      </c>
+      <c r="AG24">
+        <v>53971594.00208335</v>
+      </c>
+      <c r="AH24">
+        <v>48652278.24625001</v>
+      </c>
+      <c r="AI24">
+        <v>43332962.49041667</v>
+      </c>
+      <c r="AJ24">
+        <v>38013646.73458333</v>
+      </c>
+      <c r="AK24">
+        <v>32694330.97875</v>
+      </c>
+      <c r="AL24">
         <v>29061627.53666667</v>
       </c>
-      <c r="AL22">
+      <c r="AM24">
         <v>25428924.09458333</v>
       </c>
-      <c r="AM22">
+      <c r="AN24">
         <v>21796220.6525</v>
       </c>
-      <c r="AN22">
+      <c r="AO24">
         <v>18163517.21041667</v>
       </c>
-      <c r="AO22">
+      <c r="AP24">
         <v>14530813.76833333</v>
       </c>
-      <c r="AP22">
+      <c r="AQ24">
         <v>10898110.32625</v>
       </c>
-      <c r="AQ22">
+      <c r="AR24">
         <v>7265406.884166666</v>
       </c>
-      <c r="AR22">
-        <v>3632703.442083333</v>
+      <c r="AS24">
+        <v>3632703.442083333</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7854,15 +8530,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR22"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -7993,10 +8669,16 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>2833161790.824167</v>
@@ -8071,9 +8753,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>2833161790.824167</v>
@@ -8148,9 +8830,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>2833161790.824167</v>
@@ -8225,9 +8907,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>2833161790.824167</v>
@@ -8302,9 +8984,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:46">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>2833161790.824167</v>
@@ -8379,9 +9061,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:46">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7">
         <v>2833161790.824167</v>
@@ -8456,9 +9138,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:46">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>2833161790.824167</v>
@@ -8533,9 +9215,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:46">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>2833161790.824167</v>
@@ -8610,9 +9292,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:46">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>2833161790.824167</v>
@@ -8687,9 +9369,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:46">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>2833161790.824167</v>
@@ -8764,9 +9446,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:46">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>2833161790.824167</v>
@@ -8841,9 +9523,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>2833161790.824167</v>
@@ -8918,9 +9600,9 @@
         <v>2833161790.824167</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:46">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>2257689781.774583</v>
@@ -8995,9 +9677,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:46">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>2257689781.774583</v>
@@ -9072,9 +9754,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:46">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16">
         <v>2257689781.774583</v>
@@ -9149,9 +9831,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:46">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <v>2257689781.774583</v>
@@ -9226,9 +9908,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:46">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R18">
         <v>2257689781.774583</v>
@@ -9303,9 +9985,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:46">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S19">
         <v>2257689781.774583</v>
@@ -9380,9 +10062,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:46">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20">
         <v>2257689781.774583</v>
@@ -9457,9 +10139,9 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:46">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U21">
         <v>2257689781.774583</v>
@@ -9534,138 +10216,298 @@
         <v>2257689781.774583</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:46">
       <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
-        <v>2833161790.824167</v>
-      </c>
-      <c r="C22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="W22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="X22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Y22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="Z22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AA22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AB22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AC22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AD22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AE22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AF22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AG22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AH22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AI22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AJ22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AK22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AL22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AM22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AN22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AO22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AP22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AQ22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AR22">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AS22">
+        <v>2257689781.774583</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>2833161790.824167</v>
+      </c>
+      <c r="C24">
         <v>5666323581.648334</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>8499485372.4725</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>11332647163.29667</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>14165808954.12083</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>16998970744.945</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>19832132535.76917</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>22665294326.59333</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>25498456117.4175</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>28331617908.24166</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>31164779699.06583</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>33997941489.89</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>36255631271.66458</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>38513321053.43916</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>40771010835.21375</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>43028700616.98833</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>45286390398.76291</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>47544080180.53749</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>49801769962.31207</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>52059459744.08665</v>
       </c>
-      <c r="V22">
-        <v>52059459744.08665</v>
-      </c>
-      <c r="W22">
-        <v>52059459744.08665</v>
-      </c>
-      <c r="X22">
-        <v>52059459744.08665</v>
-      </c>
-      <c r="Y22">
-        <v>52059459744.08665</v>
-      </c>
-      <c r="Z22">
-        <v>49226297953.26249</v>
-      </c>
-      <c r="AA22">
-        <v>46393136162.43832</v>
-      </c>
-      <c r="AB22">
-        <v>43559974371.61416</v>
-      </c>
-      <c r="AC22">
-        <v>40726812580.78999</v>
-      </c>
-      <c r="AD22">
-        <v>37893650789.96583</v>
-      </c>
-      <c r="AE22">
-        <v>35060488999.14166</v>
-      </c>
-      <c r="AF22">
-        <v>32227327208.31749</v>
-      </c>
-      <c r="AG22">
-        <v>29394165417.49333</v>
-      </c>
-      <c r="AH22">
-        <v>26561003626.66916</v>
-      </c>
-      <c r="AI22">
-        <v>23727841835.845</v>
-      </c>
-      <c r="AJ22">
-        <v>20894680045.02083</v>
-      </c>
-      <c r="AK22">
+      <c r="V24">
+        <v>54317149525.86124</v>
+      </c>
+      <c r="W24">
+        <v>54317149525.86124</v>
+      </c>
+      <c r="X24">
+        <v>54317149525.86124</v>
+      </c>
+      <c r="Y24">
+        <v>54317149525.86124</v>
+      </c>
+      <c r="Z24">
+        <v>51483987735.03707</v>
+      </c>
+      <c r="AA24">
+        <v>48650825944.21291</v>
+      </c>
+      <c r="AB24">
+        <v>45817664153.38874</v>
+      </c>
+      <c r="AC24">
+        <v>42984502362.56458</v>
+      </c>
+      <c r="AD24">
+        <v>40151340571.74041</v>
+      </c>
+      <c r="AE24">
+        <v>37318178780.91624</v>
+      </c>
+      <c r="AF24">
+        <v>34485016990.09208</v>
+      </c>
+      <c r="AG24">
+        <v>31651855199.26791</v>
+      </c>
+      <c r="AH24">
+        <v>28818693408.44374</v>
+      </c>
+      <c r="AI24">
+        <v>25985531617.61958</v>
+      </c>
+      <c r="AJ24">
+        <v>23152369826.79541</v>
+      </c>
+      <c r="AK24">
+        <v>20319208035.97125</v>
+      </c>
+      <c r="AL24">
         <v>18061518254.19667</v>
       </c>
-      <c r="AL22">
+      <c r="AM24">
         <v>15803828472.42208</v>
       </c>
-      <c r="AM22">
+      <c r="AN24">
         <v>13546138690.6475</v>
       </c>
-      <c r="AN22">
+      <c r="AO24">
         <v>11288448908.87292</v>
       </c>
-      <c r="AO22">
+      <c r="AP24">
         <v>9030759127.098333</v>
       </c>
-      <c r="AP22">
+      <c r="AQ24">
         <v>6773069345.32375</v>
       </c>
-      <c r="AQ22">
+      <c r="AR24">
         <v>4515379563.549167</v>
       </c>
-      <c r="AR22">
-        <v>2257689781.774583</v>
+      <c r="AS24">
+        <v>2257689781.774583</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>